<commit_message>
Add news.exls & update code
</commit_message>
<xml_diff>
--- a/test_xlsx.xlsx
+++ b/test_xlsx.xlsx
@@ -83,7 +83,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general" vertical="bottom"/>
     </xf>
@@ -102,18 +102,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="general" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="general" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="general" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -129,18 +117,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="general" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="general" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="general" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -513,94 +489,95 @@
   </sheetPr>
   <dimension ref="A1:E74"/>
   <sheetViews>
-    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A64" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D77" activeCellId="0" sqref="D77"/>
+    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="0" outlineLevelRow="0"/>
   <cols>
-    <col width="8.539999999999999" customWidth="1" style="10" min="1" max="1"/>
-    <col width="20" customWidth="1" style="11" min="2" max="2"/>
-    <col width="20" customWidth="1" style="10" min="3" max="3"/>
-    <col width="50" customWidth="1" style="11" min="4" max="5"/>
+    <col width="8.539999999999999" customWidth="1" style="6" min="1" max="1"/>
+    <col width="20" customWidth="1" style="7" min="2" max="2"/>
+    <col width="20" customWidth="1" style="6" min="3" max="3"/>
+    <col width="50" customWidth="1" style="7" min="4" max="4"/>
+    <col width="50" customWidth="1" style="6" min="5" max="5"/>
   </cols>
   <sheetData>
-    <row r="1" ht="14.9" customHeight="1" s="12">
-      <c r="A1" s="13" t="inlineStr">
+    <row r="1" ht="14.9" customHeight="1" s="8">
+      <c r="A1" s="9" t="inlineStr">
         <is>
           <t>№</t>
         </is>
       </c>
-      <c r="B1" s="14" t="inlineStr">
+      <c r="B1" s="10" t="inlineStr">
         <is>
           <t>Имя запроса</t>
         </is>
       </c>
-      <c r="C1" s="15" t="inlineStr">
+      <c r="C1" s="11" t="inlineStr">
         <is>
           <t>Дата</t>
         </is>
       </c>
-      <c r="D1" s="14" t="inlineStr">
+      <c r="D1" s="10" t="inlineStr">
         <is>
           <t>URL объявления</t>
         </is>
       </c>
-      <c r="E1" s="16" t="inlineStr">
+      <c r="E1" s="9" t="inlineStr">
         <is>
           <t>Описание</t>
         </is>
       </c>
     </row>
-    <row r="2" ht="28.35" customHeight="1" s="12">
-      <c r="A2" s="10" t="inlineStr">
+    <row r="2">
+      <c r="A2" s="0" t="inlineStr">
         <is>
           <t>1</t>
         </is>
       </c>
-      <c r="B2" s="11" t="inlineStr">
+      <c r="B2" s="0" t="inlineStr">
         <is>
           <t>степная черепаха</t>
         </is>
       </c>
-      <c r="C2" s="10" t="inlineStr">
+      <c r="C2" s="0" t="inlineStr">
         <is>
           <t>13 июля 2022 г.</t>
         </is>
       </c>
-      <c r="D2" s="11" t="inlineStr">
+      <c r="D2" s="0" t="inlineStr">
         <is>
           <t>https://www.olx.kz/d/obyavlenie/stepnaya-cherepaha-IDmFCb6.html#9f61610c90</t>
         </is>
       </c>
-      <c r="E2" s="11" t="inlineStr">
+      <c r="E2" s="0" t="inlineStr">
         <is>
           <t>Продам Степная черепаха. Цена-7000</t>
         </is>
       </c>
     </row>
-    <row r="3" ht="162.65" customHeight="1" s="12">
-      <c r="A3" s="10" t="inlineStr">
+    <row r="3">
+      <c r="A3" s="0" t="inlineStr">
         <is>
           <t>2</t>
         </is>
       </c>
-      <c r="B3" s="11" t="inlineStr">
+      <c r="B3" s="0" t="inlineStr">
         <is>
           <t>среднеазиатская черепаха</t>
         </is>
       </c>
-      <c r="C3" s="10" t="inlineStr">
-        <is>
-          <t>25 July 2022 г.</t>
-        </is>
-      </c>
-      <c r="D3" s="11" t="inlineStr">
+      <c r="C3" s="0" t="inlineStr">
+        <is>
+          <t>25 июля 2022 г.</t>
+        </is>
+      </c>
+      <c r="D3" s="0" t="inlineStr">
         <is>
           <t>https://www.olx.kz/d/obyavlenie/suhoputnaya-sredneaziatskaya-cherepaha-IDmmd8S.html#a4015077a7;promoted</t>
         </is>
       </c>
-      <c r="E3" s="11" t="inlineStr">
+      <c r="E3" s="0" t="inlineStr">
         <is>
           <t>Среднеазиатская черепаха это дикое животное, не предназначенное для жизни в домашних условиях. 
 Чтобы черепаха хотя бы не болела у вас дома, ей нужна специальная УФ лампа и лампа для прогрева, а также правильное питание, витамины и кальций. 
@@ -610,28 +587,28 @@
         </is>
       </c>
     </row>
-    <row r="4" ht="431.3" customHeight="1" s="12">
-      <c r="A4" s="10" t="inlineStr">
+    <row r="4">
+      <c r="A4" s="0" t="inlineStr">
         <is>
           <t>3</t>
         </is>
       </c>
-      <c r="B4" s="11" t="inlineStr">
+      <c r="B4" s="0" t="inlineStr">
         <is>
           <t>среднеазиатская черепаха</t>
         </is>
       </c>
-      <c r="C4" s="10" t="inlineStr">
-        <is>
-          <t>25 July 2022 г.</t>
-        </is>
-      </c>
-      <c r="D4" s="11" t="inlineStr">
+      <c r="C4" s="0" t="inlineStr">
+        <is>
+          <t>25 июля 2022 г.</t>
+        </is>
+      </c>
+      <c r="D4" s="0" t="inlineStr">
         <is>
           <t>https://www.olx.kz/d/obyavlenie/suhoputnaya-sredneaziatskaya-cherepaha-IDmmd8S.html#a4015077a7</t>
         </is>
       </c>
-      <c r="E4" s="11" t="inlineStr">
+      <c r="E4" s="0" t="inlineStr">
         <is>
           <t>Среднеазиатская черепаха это дикое животное, не предназначенное для жизни в домашних условиях. 
 Чтобы черепаха хотя бы не болела у вас дома, ей нужна специальная УФ лампа и лампа для прогрева, а также правильное питание, витамины и кальций. 
@@ -641,28 +618,28 @@
         </is>
       </c>
     </row>
-    <row r="5" ht="673.1" customHeight="1" s="12">
-      <c r="A5" s="10" t="inlineStr">
+    <row r="5">
+      <c r="A5" s="0" t="inlineStr">
         <is>
           <t>4</t>
         </is>
       </c>
-      <c r="B5" s="11" t="inlineStr">
+      <c r="B5" s="0" t="inlineStr">
         <is>
           <t>среднеазиатская черепаха</t>
         </is>
       </c>
-      <c r="C5" s="10" t="inlineStr">
+      <c r="C5" s="0" t="inlineStr">
         <is>
           <t>12 июля 2022 г.</t>
         </is>
       </c>
-      <c r="D5" s="11" t="inlineStr">
+      <c r="D5" s="0" t="inlineStr">
         <is>
           <t>https://www.olx.kz/d/obyavlenie/sredneaziatskaya-suhoputnaya-cherepaha-IDcacJo.html#a4015077a7</t>
         </is>
       </c>
-      <c r="E5" s="11" t="inlineStr">
+      <c r="E5" s="0" t="inlineStr">
         <is>
           <t>Среднеазиатских сухопутных Черепашек размер С ДЕТСКУЮ ЛАДОШКУ ! Окрас панциря от Оливкового до Насыщенно Древесного! Фото реальные - БЕЗ ФОТОШОПА !!! Количество ограниченно- занесены в Красную книгу.
 Среди рептилий, пожалуй, это самый распространенный представитель, которого с удовольствием многие содержат в домашних условиях. Среднеазиатская сухопутная черепаха очень интересное животное, отличающееся своей медлительностью, нерасторопностью, но в тоже время, обладающая каким-то особым обаянием. Свое название среднеазиатская черепаха получила неслучайно, так как природной средой ее обитания являются многие территории Средней Азии – Казахстан, Иран, Афганистан, Пакистан, северо-западная часть Индии.
@@ -677,28 +654,28 @@
         </is>
       </c>
     </row>
-    <row r="6" ht="28.35" customHeight="1" s="12">
-      <c r="A6" s="10" t="inlineStr">
+    <row r="6">
+      <c r="A6" s="0" t="inlineStr">
         <is>
           <t>5</t>
         </is>
       </c>
-      <c r="B6" s="11" t="inlineStr">
+      <c r="B6" s="0" t="inlineStr">
         <is>
           <t>среднеазиатская черепаха</t>
         </is>
       </c>
-      <c r="C6" s="10" t="inlineStr">
+      <c r="C6" s="0" t="inlineStr">
         <is>
           <t>12 июля 2022 г.</t>
         </is>
       </c>
-      <c r="D6" s="11" t="inlineStr">
+      <c r="D6" s="0" t="inlineStr">
         <is>
           <t>https://www.olx.kz/d/obyavlenie/cherepaha-suhoputnaya-sredneaziatskaya-IDkAkve.html#a4015077a7</t>
         </is>
       </c>
-      <c r="E6" s="11" t="inlineStr">
+      <c r="E6" s="0" t="inlineStr">
         <is>
           <t>Молодые черепашки, размер около 10-13см в диаметре. 
 Есть всё необходимое для их содержания 
@@ -713,814 +690,815 @@
         </is>
       </c>
     </row>
-    <row r="7" ht="28.35" customHeight="1" s="12">
-      <c r="A7" s="10" t="inlineStr">
+    <row r="7">
+      <c r="A7" s="0" t="inlineStr">
         <is>
           <t>6</t>
         </is>
       </c>
-      <c r="B7" s="11" t="inlineStr">
+      <c r="B7" s="0" t="inlineStr">
         <is>
           <t>рога сайгака</t>
         </is>
       </c>
-      <c r="C7" s="10" t="inlineStr">
-        <is>
-          <t>25 July 2022 г.</t>
-        </is>
-      </c>
-      <c r="D7" s="11" t="inlineStr">
+      <c r="C7" s="0" t="inlineStr">
+        <is>
+          <t>25 июля 2022 г.</t>
+        </is>
+      </c>
+      <c r="D7" s="0" t="inlineStr">
         <is>
           <t>https://www.olx.kz/d/obyavlenie/prodam-rog-saygaka-IDmIIPW.html#b2bd53438d</t>
         </is>
       </c>
-      <c r="E7" s="11" t="inlineStr">
-        <is>
-          <t>Продам  один рог сайгака в хорошем состоянии писать вацап или звонить олх не читаю</t>
-        </is>
-      </c>
-    </row>
-    <row r="8" ht="28.35" customHeight="1" s="12">
-      <c r="A8" s="10" t="inlineStr">
+      <c r="E7" s="0" t="inlineStr">
+        <is>
+          <t>Продам  сувенирный один рог сайгака в хорошем состоянии писать вацап или звонить олх не читаю</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="0" t="inlineStr">
         <is>
           <t>7</t>
         </is>
       </c>
-      <c r="B8" s="11" t="inlineStr">
+      <c r="B8" s="0" t="inlineStr">
         <is>
           <t>рога сайгака</t>
         </is>
       </c>
-      <c r="C8" s="10" t="inlineStr">
+      <c r="C8" s="0" t="inlineStr">
         <is>
           <t>18 июля 2022 г.</t>
         </is>
       </c>
-      <c r="D8" s="11" t="inlineStr">
+      <c r="D8" s="0" t="inlineStr">
         <is>
           <t>https://www.olx.kz/d/obyavlenie/prodam-roga-saygaka-IDmGSi6.html#b2bd53438d</t>
         </is>
       </c>
-      <c r="E8" s="11" t="inlineStr">
+      <c r="E8" s="0" t="inlineStr">
         <is>
           <t>Продам рога сайгака , в отличном состояний все вопросы по телефону или в олх</t>
         </is>
       </c>
     </row>
-    <row r="9" ht="28.35" customHeight="1" s="12">
-      <c r="A9" s="10" t="inlineStr">
+    <row r="9">
+      <c r="A9" s="0" t="inlineStr">
         <is>
           <t>8</t>
         </is>
       </c>
-      <c r="B9" s="11" t="inlineStr">
+      <c r="B9" s="0" t="inlineStr">
         <is>
           <t>рога сайгака</t>
         </is>
       </c>
-      <c r="C9" s="10" t="inlineStr">
+      <c r="C9" s="0" t="inlineStr">
         <is>
           <t>18 июля 2022 г.</t>
         </is>
       </c>
-      <c r="D9" s="11" t="inlineStr">
+      <c r="D9" s="0" t="inlineStr">
         <is>
           <t>https://www.olx.kz/d/obyavlenie/roga-saygaka-IDmGOI2.html#b2bd53438d</t>
         </is>
       </c>
-      <c r="E9" s="11" t="inlineStr">
+      <c r="E9" s="0" t="inlineStr">
         <is>
           <t>Рога сайгака в хорошем состоянии , не сломанные …</t>
         </is>
       </c>
     </row>
-    <row r="10" ht="28.35" customHeight="1" s="12">
-      <c r="A10" s="10" t="inlineStr">
+    <row r="10">
+      <c r="A10" s="0" t="inlineStr">
         <is>
           <t>9</t>
         </is>
       </c>
-      <c r="B10" s="11" t="inlineStr">
+      <c r="B10" s="0" t="inlineStr">
         <is>
           <t>рога сайгака</t>
         </is>
       </c>
-      <c r="C10" s="10" t="inlineStr">
+      <c r="C10" s="0" t="inlineStr">
         <is>
           <t>13 июля 2022 г.</t>
         </is>
       </c>
-      <c r="D10" s="11" t="inlineStr">
+      <c r="D10" s="0" t="inlineStr">
         <is>
           <t>https://www.olx.kz/d/obyavlenie/roga-saygaka-IDmFyPY.html#b2bd53438d</t>
         </is>
       </c>
-      <c r="E10" s="11" t="inlineStr">
+      <c r="E10" s="0" t="inlineStr">
         <is>
           <t>Продаются рога сайгака сувенирный и лакированный, в очень хорошем состоянии.ееее</t>
         </is>
       </c>
     </row>
-    <row r="11" ht="55.2" customHeight="1" s="12">
-      <c r="A11" s="10" t="inlineStr">
+    <row r="11">
+      <c r="A11" s="0" t="inlineStr">
         <is>
           <t>10</t>
         </is>
       </c>
-      <c r="B11" s="11" t="inlineStr">
+      <c r="B11" s="0" t="inlineStr">
         <is>
           <t>рога сайгака</t>
         </is>
       </c>
-      <c r="C11" s="10" t="inlineStr">
+      <c r="C11" s="0" t="inlineStr">
         <is>
           <t>05 июля 2022 г.</t>
         </is>
       </c>
-      <c r="D11" s="11" t="inlineStr">
+      <c r="D11" s="0" t="inlineStr">
         <is>
           <t>https://www.olx.kz/d/obyavlenie/prodam-rog-saygaka-15000-IDmD9Cs.html#b2bd53438d</t>
         </is>
       </c>
-      <c r="E11" s="11" t="inlineStr">
+      <c r="E11" s="0" t="inlineStr">
         <is>
           <t>Продам один рог Сайгака  в отличном состояние 15000т звонить на номер 87789069623</t>
         </is>
       </c>
     </row>
-    <row r="12" ht="55.2" customHeight="1" s="12">
-      <c r="A12" s="10" t="inlineStr">
+    <row r="12">
+      <c r="A12" s="0" t="inlineStr">
         <is>
           <t>11</t>
         </is>
       </c>
-      <c r="B12" s="11" t="inlineStr">
+      <c r="B12" s="0" t="inlineStr">
         <is>
           <t>рога сайгака</t>
         </is>
       </c>
-      <c r="C12" s="10" t="inlineStr">
+      <c r="C12" s="0" t="inlineStr">
         <is>
           <t>03 июля 2022 г.</t>
         </is>
       </c>
-      <c r="D12" s="11" t="inlineStr">
+      <c r="D12" s="0" t="inlineStr">
         <is>
           <t>https://www.olx.kz/d/obyavlenie/prodam-roga-saygaka-i-korovy-IDmCmNW.html#b2bd53438d</t>
         </is>
       </c>
-      <c r="E12" s="11" t="inlineStr">
+      <c r="E12" s="0" t="inlineStr">
         <is>
           <t>Продам рога сайгака, коровы. Времён СССР. Две пары сайгака по 10000 тысяч тенге каждая, коровы 1 большой рог по 5000 тысяч тенге, 5 шт по 2500 тысяч тенге каждая. Телефон для связи: +77713794580</t>
         </is>
       </c>
     </row>
-    <row r="13" ht="28.35" customHeight="1" s="12">
-      <c r="A13" s="10" t="inlineStr">
+    <row r="13">
+      <c r="A13" s="0" t="inlineStr">
         <is>
           <t>12</t>
         </is>
       </c>
-      <c r="B13" s="11" t="inlineStr">
+      <c r="B13" s="0" t="inlineStr">
         <is>
           <t>рога сайгака</t>
         </is>
       </c>
-      <c r="C13" s="10" t="inlineStr">
+      <c r="C13" s="0" t="inlineStr">
         <is>
           <t>03 июля 2022 г.</t>
         </is>
       </c>
-      <c r="D13" s="11" t="inlineStr">
+      <c r="D13" s="0" t="inlineStr">
         <is>
           <t>https://www.olx.kz/d/obyavlenie/prodayu-roga-saygaka-za-10500-IDmCdSp.html#b2bd53438d</t>
         </is>
       </c>
-      <c r="E13" s="11" t="inlineStr">
+      <c r="E13" s="0" t="inlineStr">
         <is>
           <t>Продаются рога сайгака в очень хорошем состоянии. Длина рог 30 см. Возраст даже не могу сказать. Достались от деда. Относились антиквариату бережно.  Торг минимальный.</t>
         </is>
       </c>
     </row>
-    <row r="14" ht="41.75" customHeight="1" s="12">
-      <c r="A14" s="10" t="inlineStr">
+    <row r="14">
+      <c r="A14" s="0" t="inlineStr">
         <is>
           <t>13</t>
         </is>
       </c>
-      <c r="B14" s="11" t="inlineStr">
-        <is>
-          <t>продам черепаху</t>
-        </is>
-      </c>
-      <c r="C14" s="10" t="inlineStr">
+      <c r="B14" s="0" t="inlineStr">
+        <is>
+          <t>продам черепаху</t>
+        </is>
+      </c>
+      <c r="C14" s="0" t="inlineStr">
         <is>
           <t>29 июня 2022 г.</t>
         </is>
       </c>
-      <c r="D14" s="11" t="inlineStr">
+      <c r="D14" s="0" t="inlineStr">
         <is>
           <t>https://www.olx.kz/d/obyavlenie/prodam-cherepahu-vsego-1000-tenge-IDhTpbn.html#729a76a98a</t>
         </is>
       </c>
-      <c r="E14" s="11" t="inlineStr">
+      <c r="E14" s="0" t="inlineStr">
         <is>
           <t>Состояние отличное. 87052556503 или 87011050397</t>
         </is>
       </c>
     </row>
-    <row r="15" ht="55.2" customHeight="1" s="12">
-      <c r="A15" s="10" t="inlineStr">
+    <row r="15">
+      <c r="A15" s="0" t="inlineStr">
         <is>
           <t>14</t>
         </is>
       </c>
-      <c r="B15" s="11" t="inlineStr">
-        <is>
-          <t>продам черепаху</t>
-        </is>
-      </c>
-      <c r="C15" s="10" t="inlineStr">
+      <c r="B15" s="0" t="inlineStr">
+        <is>
+          <t>продам черепаху</t>
+        </is>
+      </c>
+      <c r="C15" s="0" t="inlineStr">
         <is>
           <t>29 июня 2022 г.</t>
         </is>
       </c>
-      <c r="D15" s="11" t="inlineStr">
+      <c r="D15" s="0" t="inlineStr">
         <is>
           <t>https://www.olx.kz/d/obyavlenie/prodam-cherepahu-v-vide-podushki-suvenira-IDkjfDH.html#729a76a98a</t>
         </is>
       </c>
-      <c r="E15" s="11" t="inlineStr">
+      <c r="E15" s="0" t="inlineStr">
         <is>
           <t>Продам черепаху в виде подушки сувенира можно использовать как подушку или сувенир очень мягкая удобная</t>
         </is>
       </c>
     </row>
-    <row r="16" ht="55.2" customHeight="1" s="12">
-      <c r="A16" s="10" t="inlineStr">
+    <row r="16">
+      <c r="A16" s="0" t="inlineStr">
         <is>
           <t>15</t>
         </is>
       </c>
-      <c r="B16" s="11" t="inlineStr">
-        <is>
-          <t>продам черепаху</t>
-        </is>
-      </c>
-      <c r="C16" s="10" t="inlineStr">
+      <c r="B16" s="0" t="inlineStr">
+        <is>
+          <t>продам черепаху</t>
+        </is>
+      </c>
+      <c r="C16" s="0" t="inlineStr">
         <is>
           <t>29 июня 2022 г.</t>
         </is>
       </c>
-      <c r="D16" s="11" t="inlineStr">
+      <c r="D16" s="0" t="inlineStr">
         <is>
           <t>https://www.olx.kz/d/obyavlenie/prodam-cherepahu-motocherepaha-zaschita-dlya-moto-ekipirovka-IDkGcEF.html#729a76a98a</t>
         </is>
       </c>
-      <c r="E16" s="11" t="inlineStr">
+      <c r="E16" s="0" t="inlineStr">
         <is>
           <t>Продам мото черепаху большого размера фирмы Vega Черепаха, защита локтя, защита спины, поясницы, грудной клетки, полная защита [VEGA] Есть торг возможна отправка в любую точку kz! Состояние Б/У!</t>
         </is>
       </c>
     </row>
-    <row r="17" ht="95.5" customHeight="1" s="12">
-      <c r="A17" s="10" t="inlineStr">
+    <row r="17">
+      <c r="A17" s="0" t="inlineStr">
         <is>
           <t>16</t>
         </is>
       </c>
-      <c r="B17" s="11" t="inlineStr">
-        <is>
-          <t>продам черепаху</t>
-        </is>
-      </c>
-      <c r="C17" s="10" t="inlineStr">
+      <c r="B17" s="0" t="inlineStr">
+        <is>
+          <t>продам черепаху</t>
+        </is>
+      </c>
+      <c r="C17" s="0" t="inlineStr">
         <is>
           <t>28 июня 2022 г.</t>
         </is>
       </c>
-      <c r="D17" s="11" t="inlineStr">
+      <c r="D17" s="0" t="inlineStr">
         <is>
           <t>https://www.olx.kz/d/obyavlenie/prodam-cherepahu-bolshuyu-IDmd2YO.html#729a76a98a</t>
         </is>
       </c>
-      <c r="E17" s="11" t="inlineStr">
+      <c r="E17" s="0" t="inlineStr">
         <is>
           <t>Продам сухопутныю черепаху .Примерно 15 см .Самовывоз. По всем другим вопросам пишите на ватсап.не одыкватных прошу не беспокоить.Только в хорошим руки.</t>
         </is>
       </c>
     </row>
-    <row r="18" ht="41.75" customHeight="1" s="12">
-      <c r="A18" s="10" t="inlineStr">
+    <row r="18">
+      <c r="A18" s="0" t="inlineStr">
         <is>
           <t>17</t>
         </is>
       </c>
-      <c r="B18" s="11" t="inlineStr">
-        <is>
-          <t>продам черепаху</t>
-        </is>
-      </c>
-      <c r="C18" s="10" t="inlineStr">
+      <c r="B18" s="0" t="inlineStr">
+        <is>
+          <t>продам черепаху</t>
+        </is>
+      </c>
+      <c r="C18" s="0" t="inlineStr">
         <is>
           <t>27 июня 2022 г.</t>
         </is>
       </c>
-      <c r="D18" s="11" t="inlineStr">
+      <c r="D18" s="0" t="inlineStr">
         <is>
           <t>https://www.olx.kz/d/obyavlenie/vnimanie-prodam-krasnouhuyu-cherepahu-kupi-i-podari-rebenku-radost-IDl1pk4.html#729a76a98a</t>
         </is>
       </c>
-      <c r="E18" s="11" t="inlineStr">
+      <c r="E18" s="0" t="inlineStr">
         <is>
           <t>Продам НЕДОРОГО красноухую черепаху. Черепаха дрессированная- не гавкает, не мяукает, не линяет, не портит мебель, не гадит в тапки, не шумит, не бегает, не надо выгуливать, ест раз в 2-3 дня - а это то что нужно Вам!!! Ест  сырую рыбу, мясо, морковь, огурцы, зелень.  Живут до 40-50 лет. Достанутся ещё и внукам!!! Сделайте выгодную покупку!!!</t>
         </is>
       </c>
     </row>
-    <row r="19" ht="28.35" customHeight="1" s="12">
-      <c r="A19" s="10" t="inlineStr">
+    <row r="19">
+      <c r="A19" s="0" t="inlineStr">
         <is>
           <t>18</t>
         </is>
       </c>
-      <c r="B19" s="11" t="inlineStr">
-        <is>
-          <t>продам черепаху</t>
-        </is>
-      </c>
-      <c r="C19" s="10" t="inlineStr">
-        <is>
-          <t>26 июня 2022 г.</t>
-        </is>
-      </c>
-      <c r="D19" s="11" t="inlineStr">
-        <is>
-          <t>https://www.olx.kz/d/obyavlenie/prodam-cherepahu-suhoputnuyu-IDmApNA.html#729a76a98a</t>
-        </is>
-      </c>
-      <c r="E19" s="11" t="inlineStr">
-        <is>
-          <t>Продам сухопутную черепашку ,возрост около 10лет
-Питается фруктами и овощами.
-Цена окончательная</t>
-        </is>
-      </c>
-    </row>
-    <row r="20" ht="28.35" customHeight="1" s="12">
-      <c r="A20" s="10" t="inlineStr">
+      <c r="B19" s="0" t="inlineStr">
+        <is>
+          <t>продам черепаху</t>
+        </is>
+      </c>
+      <c r="C19" s="0" t="inlineStr">
+        <is>
+          <t>27 July 2022 г.</t>
+        </is>
+      </c>
+      <c r="D19" s="0" t="inlineStr">
+        <is>
+          <t>https://www.olx.kz/d/obyavlenie/srochno-prodam-cherepahu-IDmISKn.html#fe43e5f20a</t>
+        </is>
+      </c>
+      <c r="E19" s="0" t="inlineStr">
+        <is>
+          <t>Срочно Продам черепаху красноухая с аквариумом 35литров, все вопросы по указанному номеру на фото</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="0" t="inlineStr">
         <is>
           <t>19</t>
         </is>
       </c>
-      <c r="B20" s="11" t="inlineStr">
-        <is>
-          <t>продам черепаху</t>
-        </is>
-      </c>
-      <c r="C20" s="10" t="inlineStr">
-        <is>
-          <t>26 июня 2022 г.</t>
-        </is>
-      </c>
-      <c r="D20" s="11" t="inlineStr">
-        <is>
-          <t>https://www.olx.kz/d/obyavlenie/prodam-cherepahu-IDmAfDd.html#729a76a98a</t>
-        </is>
-      </c>
-      <c r="E20" s="11" t="inlineStr">
-        <is>
-          <t>Продам черепаху. Продам черепаху. Продам черепаху. Продам черепаху. Продам черепаху.</t>
-        </is>
-      </c>
-    </row>
-    <row r="21" ht="149.25" customHeight="1" s="12">
-      <c r="A21" s="10" t="inlineStr">
+      <c r="B20" s="0" t="inlineStr">
+        <is>
+          <t>продам черепаху</t>
+        </is>
+      </c>
+      <c r="C20" s="0" t="inlineStr">
+        <is>
+          <t>25 июля 2022 г.</t>
+        </is>
+      </c>
+      <c r="D20" s="0" t="inlineStr">
+        <is>
+          <t>https://www.olx.kz/d/obyavlenie/prodam-klevuyu-domashnyuyu-cherepahu-IDkkx0i.html#fe43e5f20a;promoted</t>
+        </is>
+      </c>
+      <c r="E20" s="0" t="inlineStr">
+        <is>
+          <t>Продается обычная степная черепашка,любит листья салата,одуванчика,морковь ,капусту.  Отличное домашнее животное. Ручные черепашки ,людей не боятся. Есть мальчики и девочки. Находимся  нижней части города. Возможно доставка за отдельную плату. МАЛЕНЬКАЯ ЧЕРЕПАХА 10 000ТГ. СРЕДЕЯЯ 7000ТГ. БОЛЬШАЯ 5000тг.</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="0" t="inlineStr">
         <is>
           <t>20</t>
         </is>
       </c>
-      <c r="B21" s="11" t="inlineStr">
-        <is>
-          <t>продам черепаху</t>
-        </is>
-      </c>
-      <c r="C21" s="10" t="inlineStr">
-        <is>
-          <t>25 July 2022 г.</t>
-        </is>
-      </c>
-      <c r="D21" s="11" t="inlineStr">
-        <is>
-          <t>https://www.olx.kz/d/obyavlenie/prodam-klevuyu-domashnyuyu-cherepahu-IDkkx0i.html#fe43e5f20a;promoted</t>
-        </is>
-      </c>
-      <c r="E21" s="11" t="inlineStr">
+      <c r="B21" s="0" t="inlineStr">
+        <is>
+          <t>продам черепаху</t>
+        </is>
+      </c>
+      <c r="C21" s="0" t="inlineStr">
+        <is>
+          <t>25 июля 2022 г.</t>
+        </is>
+      </c>
+      <c r="D21" s="0" t="inlineStr">
+        <is>
+          <t>https://www.olx.kz/d/obyavlenie/srochno-prodam-cherepahu-cherepaha-domashnyaya-IDmccCo.html#fe43e5f20a</t>
+        </is>
+      </c>
+      <c r="E21" s="0" t="inlineStr">
+        <is>
+          <t>Домашняя степная маленькая черепаха. Довольно активная. питается травой, одуванчиками,огурцами,морковкой,листьями салата.
+отличный подарок для ребенка,да и в общем домашнее животное)
+продаем по причине переезда
+СРОЧНО</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="0" t="inlineStr">
+        <is>
+          <t>21</t>
+        </is>
+      </c>
+      <c r="B22" s="0" t="inlineStr">
+        <is>
+          <t>продам черепаху</t>
+        </is>
+      </c>
+      <c r="C22" s="0" t="inlineStr">
+        <is>
+          <t>25 июля 2022 г.</t>
+        </is>
+      </c>
+      <c r="D22" s="0" t="inlineStr">
+        <is>
+          <t>https://www.olx.kz/d/obyavlenie/prodam-cherepahu-6-let-IDmIIaP.html#fe43e5f20a</t>
+        </is>
+      </c>
+      <c r="E22" s="0" t="inlineStr">
+        <is>
+          <t>Продам черепаху в хорошие руки, черепахе 6 лет, здоровая. В еде не превередливая.</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="0" t="inlineStr">
+        <is>
+          <t>22</t>
+        </is>
+      </c>
+      <c r="B23" s="0" t="inlineStr">
+        <is>
+          <t>продам черепаху</t>
+        </is>
+      </c>
+      <c r="C23" s="0" t="inlineStr">
+        <is>
+          <t>25 июля 2022 г.</t>
+        </is>
+      </c>
+      <c r="D23" s="0" t="inlineStr">
+        <is>
+          <t>https://www.olx.kz/d/obyavlenie/prodam-klevuyu-domashnyuyu-cherepahu-IDkkx0i.html#fe43e5f20a</t>
+        </is>
+      </c>
+      <c r="E23" s="0" t="inlineStr">
         <is>
           <t>Продается обычная степная черепашка,любит листья салата,одуванчика,морковь ,капусту.  Отличное домашнее животное. Ручные черепашки ,людей не боятся. Есть мальчики и девочки. Находимся  нижней части города. Возможно доставка за отдельную плату. МАЛЕНЬКАЯ ЧЕРЕПАХА 10 000ТГ. СРЕДЕЯЯ 7000ТГ. БОЛЬШАЯ 5000тг.</t>
         </is>
       </c>
     </row>
-    <row r="22" ht="28.35" customHeight="1" s="12">
-      <c r="A22" s="10" t="inlineStr">
-        <is>
-          <t>21</t>
-        </is>
-      </c>
-      <c r="B22" s="11" t="inlineStr">
-        <is>
-          <t>продам черепаху</t>
-        </is>
-      </c>
-      <c r="C22" s="10" t="inlineStr">
-        <is>
-          <t>25 July 2022 г.</t>
-        </is>
-      </c>
-      <c r="D22" s="11" t="inlineStr">
-        <is>
-          <t>https://www.olx.kz/d/obyavlenie/prodam-cherepahu-6-let-IDmIIaP.html#fe43e5f20a</t>
-        </is>
-      </c>
-      <c r="E22" s="17" t="inlineStr">
-        <is>
-          <t>Продам черепаху в хорошие руки, черепахе 6 лет, здоровая. В еде не превередливая.</t>
-        </is>
-      </c>
-    </row>
-    <row r="23" ht="55.2" customHeight="1" s="12">
-      <c r="A23" s="10" t="inlineStr">
-        <is>
-          <t>22</t>
-        </is>
-      </c>
-      <c r="B23" s="11" t="inlineStr">
-        <is>
-          <t>продам черепаху</t>
-        </is>
-      </c>
-      <c r="C23" s="10" t="inlineStr">
-        <is>
-          <t>25 July 2022 г.</t>
-        </is>
-      </c>
-      <c r="D23" s="11" t="inlineStr">
-        <is>
-          <t>https://www.olx.kz/d/obyavlenie/prodam-klevuyu-domashnyuyu-cherepahu-IDkkx0i.html#fe43e5f20a</t>
-        </is>
-      </c>
-      <c r="E23" s="11" t="inlineStr">
+    <row r="24">
+      <c r="A24" s="0" t="inlineStr">
+        <is>
+          <t>23</t>
+        </is>
+      </c>
+      <c r="B24" s="0" t="inlineStr">
+        <is>
+          <t>продам черепаху</t>
+        </is>
+      </c>
+      <c r="C24" s="0" t="inlineStr">
+        <is>
+          <t>25 июля 2022 г.</t>
+        </is>
+      </c>
+      <c r="D24" s="0" t="inlineStr">
+        <is>
+          <t>https://www.olx.kz/d/obyavlenie/prodam-klevuyu-domashnyuyu-cherepahu-IDkkx0i.html#729a76a98a;promoted</t>
+        </is>
+      </c>
+      <c r="E24" s="0" t="inlineStr">
         <is>
           <t>Продается обычная степная черепашка,любит листья салата,одуванчика,морковь ,капусту.  Отличное домашнее животное. Ручные черепашки ,людей не боятся. Есть мальчики и девочки. Находимся  нижней части города. Возможно доставка за отдельную плату. МАЛЕНЬКАЯ ЧЕРЕПАХА 10 000ТГ. СРЕДЕЯЯ 7000ТГ. БОЛЬШАЯ 5000тг.</t>
         </is>
       </c>
     </row>
-    <row r="24" ht="95.5" customHeight="1" s="12">
-      <c r="A24" s="10" t="inlineStr">
-        <is>
-          <t>23</t>
-        </is>
-      </c>
-      <c r="B24" s="11" t="inlineStr">
-        <is>
-          <t>продам черепаху</t>
-        </is>
-      </c>
-      <c r="C24" s="10" t="inlineStr">
-        <is>
-          <t>25 July 2022 г.</t>
-        </is>
-      </c>
-      <c r="D24" s="11" t="inlineStr">
-        <is>
-          <t>https://www.olx.kz/d/obyavlenie/prodam-klevuyu-domashnyuyu-cherepahu-IDkkx0i.html#729a76a98a;promoted</t>
-        </is>
-      </c>
-      <c r="E24" s="11" t="inlineStr">
-        <is>
-          <t>Продается обычная степная черепашка,любит листья салата,одуванчика,морковь ,капусту.  Отличное домашнее животное. Ручные черепашки ,людей не боятся. Есть мальчики и девочки. Находимся  нижней части города. Возможно доставка за отдельную плату. МАЛЕНЬКАЯ ЧЕРЕПАХА 10 000ТГ. СРЕДЕЯЯ 7000ТГ. БОЛЬШАЯ 5000тг.</t>
-        </is>
-      </c>
-    </row>
-    <row r="25" ht="95.5" customHeight="1" s="12">
-      <c r="A25" s="10" t="inlineStr">
+    <row r="25">
+      <c r="A25" s="0" t="inlineStr">
         <is>
           <t>24</t>
         </is>
       </c>
-      <c r="B25" s="11" t="inlineStr">
-        <is>
-          <t>продам черепаху</t>
-        </is>
-      </c>
-      <c r="C25" s="10" t="inlineStr">
+      <c r="B25" s="0" t="inlineStr">
+        <is>
+          <t>продам черепаху</t>
+        </is>
+      </c>
+      <c r="C25" s="0" t="inlineStr">
         <is>
           <t>24 июля 2022 г.</t>
         </is>
       </c>
-      <c r="D25" s="11" t="inlineStr">
+      <c r="D25" s="0" t="inlineStr">
         <is>
           <t>https://www.olx.kz/d/obyavlenie/prodam-cherepahu-IDmIsc5.html#fe43e5f20a</t>
         </is>
       </c>
-      <c r="E25" s="11" t="inlineStr">
+      <c r="E25" s="0" t="inlineStr">
         <is>
           <t>Продам черепаху водяная  красноухая вместе с аквариумом</t>
         </is>
       </c>
     </row>
-    <row r="26" ht="95.5" customHeight="1" s="12">
-      <c r="A26" s="10" t="inlineStr">
+    <row r="26">
+      <c r="A26" s="0" t="inlineStr">
         <is>
           <t>25</t>
         </is>
       </c>
-      <c r="B26" s="11" t="inlineStr">
-        <is>
-          <t>продам черепаху</t>
-        </is>
-      </c>
-      <c r="C26" s="10" t="inlineStr">
+      <c r="B26" s="0" t="inlineStr">
+        <is>
+          <t>продам черепаху</t>
+        </is>
+      </c>
+      <c r="C26" s="0" t="inlineStr">
         <is>
           <t>22 июля 2022 г.</t>
         </is>
       </c>
-      <c r="D26" s="11" t="inlineStr">
+      <c r="D26" s="0" t="inlineStr">
         <is>
           <t>https://www.olx.kz/d/obyavlenie/prodam-vodyanuyu-krasnouhuyu-cherepahu-IDmHU2l.html#fe43e5f20a</t>
         </is>
       </c>
-      <c r="E26" s="11" t="inlineStr">
+      <c r="E26" s="0" t="inlineStr">
         <is>
           <t>Продам водяную, красноухую черепаху.Активная.Длинна панцыря ≈12 см.Девочка.Любит рыбу,но не нужно акцентироваться на одной рыбе.В еде не прихотлива.Или меняю на рыбок.Варианты обмена.Интересует так же к обмену на фильтр аквариумный с компрессором.Цена  без аквариума 3000тг.С аквариумом 5000т.</t>
         </is>
       </c>
     </row>
-    <row r="27" ht="28.35" customHeight="1" s="12">
-      <c r="A27" s="10" t="inlineStr">
+    <row r="27">
+      <c r="A27" s="0" t="inlineStr">
         <is>
           <t>26</t>
         </is>
       </c>
-      <c r="B27" s="11" t="inlineStr">
-        <is>
-          <t>продам черепаху</t>
-        </is>
-      </c>
-      <c r="C27" s="10" t="inlineStr">
+      <c r="B27" s="0" t="inlineStr">
+        <is>
+          <t>продам черепаху</t>
+        </is>
+      </c>
+      <c r="C27" s="0" t="inlineStr">
         <is>
           <t>22 июля 2022 г.</t>
         </is>
       </c>
-      <c r="D27" s="11" t="inlineStr">
+      <c r="D27" s="0" t="inlineStr">
         <is>
           <t>https://www.olx.kz/d/obyavlenie/krasnouhaya-cherepaha-prodam-IDmHQYX.html#fe43e5f20a</t>
         </is>
       </c>
-      <c r="E27" s="11" t="inlineStr">
+      <c r="E27" s="0" t="inlineStr">
         <is>
           <t>Продам черепаху, уже большая, звонить по номеру +7 777 147 4308. .</t>
         </is>
       </c>
     </row>
-    <row r="28" ht="28.35" customHeight="1" s="12">
-      <c r="A28" s="10" t="inlineStr">
+    <row r="28">
+      <c r="A28" s="0" t="inlineStr">
         <is>
           <t>27</t>
         </is>
       </c>
-      <c r="B28" s="11" t="inlineStr">
-        <is>
-          <t>продам черепаху</t>
-        </is>
-      </c>
-      <c r="C28" s="10" t="inlineStr">
+      <c r="B28" s="0" t="inlineStr">
+        <is>
+          <t>продам черепаху</t>
+        </is>
+      </c>
+      <c r="C28" s="0" t="inlineStr">
         <is>
           <t>22 июля 2022 г.</t>
         </is>
       </c>
-      <c r="D28" s="11" t="inlineStr">
+      <c r="D28" s="0" t="inlineStr">
         <is>
           <t>https://www.olx.kz/d/obyavlenie/prodam-cherepahu-srochno-do-24-go-IDmHMZl.html#fe43e5f20a</t>
         </is>
       </c>
-      <c r="E28" s="11" t="inlineStr">
+      <c r="E28" s="0" t="inlineStr">
         <is>
           <t>Срочно продам черепаху. Каждый по 5000 тенге. Кушают овощи фрукты.
 Пишите звоните 87471250196</t>
         </is>
       </c>
     </row>
-    <row r="29" ht="41.75" customHeight="1" s="12">
-      <c r="A29" s="10" t="inlineStr">
+    <row r="29">
+      <c r="A29" s="0" t="inlineStr">
         <is>
           <t>28</t>
         </is>
       </c>
-      <c r="B29" s="11" t="inlineStr">
-        <is>
-          <t>продам черепаху</t>
-        </is>
-      </c>
-      <c r="C29" s="10" t="inlineStr">
+      <c r="B29" s="0" t="inlineStr">
+        <is>
+          <t>продам черепаху</t>
+        </is>
+      </c>
+      <c r="C29" s="0" t="inlineStr">
         <is>
           <t>21 июля 2022 г.</t>
         </is>
       </c>
-      <c r="D29" s="11" t="inlineStr">
+      <c r="D29" s="0" t="inlineStr">
         <is>
           <t>https://www.olx.kz/d/obyavlenie/prodam-krasnouhuyu-cherepahu-dve-20000-tg-IDmHIP5.html#fe43e5f20a</t>
         </is>
       </c>
-      <c r="E29" s="11" t="inlineStr">
+      <c r="E29" s="0" t="inlineStr">
         <is>
           <t>Продам красноухую черепаху. Одна большая 17-18 см. Второй маленький 7-8 см. Две черепахи стоит 10000 тг. Есть торг. Продаю аквариум 5000 тг. Есть торг. Номер телефона: 87027487150</t>
         </is>
       </c>
     </row>
-    <row r="30" ht="28.35" customHeight="1" s="12">
-      <c r="A30" s="10" t="inlineStr">
+    <row r="30">
+      <c r="A30" s="0" t="inlineStr">
         <is>
           <t>29</t>
         </is>
       </c>
-      <c r="B30" s="11" t="inlineStr">
-        <is>
-          <t>продам черепаху</t>
-        </is>
-      </c>
-      <c r="C30" s="10" t="inlineStr">
+      <c r="B30" s="0" t="inlineStr">
+        <is>
+          <t>продам черепаху</t>
+        </is>
+      </c>
+      <c r="C30" s="0" t="inlineStr">
         <is>
           <t>21 июля 2022 г.</t>
         </is>
       </c>
-      <c r="D30" s="11" t="inlineStr">
+      <c r="D30" s="0" t="inlineStr">
         <is>
           <t>https://www.olx.kz/d/obyavlenie/prodam-kovrik-cherepahu-IDmHI15.html#fe43e5f20a</t>
         </is>
       </c>
-      <c r="E30" s="11" t="inlineStr">
-        <is>
-          <t>Продам развивающий коврик черепаха. В хорошем состоянии. Все вопросы по телефону 87711785817</t>
-        </is>
-      </c>
-    </row>
-    <row r="31" ht="95.5" customHeight="1" s="12">
-      <c r="A31" s="10" t="inlineStr">
+      <c r="E30" s="0" t="inlineStr">
+        <is>
+          <t>Продам развивающий коврик черепаха. В хорошем состоянии. Так же  возможен обмен на мед. Все вопросы по телефону 87711785817</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="0" t="inlineStr">
         <is>
           <t>30</t>
         </is>
       </c>
-      <c r="B31" s="11" t="inlineStr">
-        <is>
-          <t>продам черепаху</t>
-        </is>
-      </c>
-      <c r="C31" s="10" t="inlineStr">
+      <c r="B31" s="0" t="inlineStr">
+        <is>
+          <t>продам черепаху</t>
+        </is>
+      </c>
+      <c r="C31" s="0" t="inlineStr">
         <is>
           <t>20 июля 2022 г.</t>
         </is>
       </c>
-      <c r="D31" s="11" t="inlineStr">
+      <c r="D31" s="0" t="inlineStr">
         <is>
           <t>https://www.olx.kz/d/obyavlenie/prodam-krasnouhie-cherepahi-IDm2mxZ.html#fe43e5f20a</t>
         </is>
       </c>
-      <c r="E31" s="11" t="inlineStr">
+      <c r="E31" s="0" t="inlineStr">
         <is>
           <t>Продам 2ух красноухих черепашек.Без аквариума и воздуха,в придачу к обоим отдам их островок.Для содержания аквариум обязателен.Кушают замороженную и живую малинку(мотыль),курицу,рыбу.Или поменяю на попугая.Обращатся на вотсап 87711727960 Возможен обмен,рассмотрю любые варианты</t>
         </is>
       </c>
     </row>
-    <row r="32" ht="243.25" customHeight="1" s="12">
-      <c r="A32" s="10" t="inlineStr">
+    <row r="32">
+      <c r="A32" s="0" t="inlineStr">
         <is>
           <t>31</t>
         </is>
       </c>
-      <c r="B32" s="11" t="inlineStr">
-        <is>
-          <t>продам черепаху</t>
-        </is>
-      </c>
-      <c r="C32" s="10" t="inlineStr">
+      <c r="B32" s="0" t="inlineStr">
+        <is>
+          <t>продам черепаху</t>
+        </is>
+      </c>
+      <c r="C32" s="0" t="inlineStr">
         <is>
           <t>19 июля 2022 г.</t>
         </is>
       </c>
-      <c r="D32" s="11" t="inlineStr">
+      <c r="D32" s="0" t="inlineStr">
         <is>
           <t>https://www.olx.kz/d/obyavlenie/prodam-cherepahu-IDmH3XU.html#fe43e5f20a</t>
         </is>
       </c>
-      <c r="E32" s="11" t="inlineStr">
+      <c r="E32" s="0" t="inlineStr">
         <is>
           <t>Продам сухопутную черепаху в добрые руки,ест капусту, купать надо 2-3раза в неделю</t>
         </is>
       </c>
     </row>
-    <row r="33" ht="28.35" customHeight="1" s="12">
-      <c r="A33" s="10" t="inlineStr">
+    <row r="33">
+      <c r="A33" s="0" t="inlineStr">
         <is>
           <t>32</t>
         </is>
       </c>
-      <c r="B33" s="11" t="inlineStr">
-        <is>
-          <t>продам черепаху</t>
-        </is>
-      </c>
-      <c r="C33" s="10" t="inlineStr">
+      <c r="B33" s="0" t="inlineStr">
+        <is>
+          <t>продам черепаху</t>
+        </is>
+      </c>
+      <c r="C33" s="0" t="inlineStr">
         <is>
           <t>19 июля 2022 г.</t>
         </is>
       </c>
-      <c r="D33" s="11" t="inlineStr">
+      <c r="D33" s="0" t="inlineStr">
         <is>
           <t>https://www.olx.kz/d/obyavlenie/prodam-malenkuyu-cherepahu-IDmH3W0.html#fe43e5f20a</t>
         </is>
       </c>
-      <c r="E33" s="11" t="inlineStr">
+      <c r="E33" s="0" t="inlineStr">
         <is>
           <t>продам маленькую сухопутную черепаху, ест капусту, купать надо 2-3раза в неделю.</t>
         </is>
       </c>
     </row>
-    <row r="34" ht="41.75" customHeight="1" s="12">
-      <c r="A34" s="10" t="inlineStr">
+    <row r="34">
+      <c r="A34" s="0" t="inlineStr">
         <is>
           <t>33</t>
         </is>
       </c>
-      <c r="B34" s="11" t="inlineStr">
-        <is>
-          <t>продам черепаху</t>
-        </is>
-      </c>
-      <c r="C34" s="10" t="inlineStr">
+      <c r="B34" s="0" t="inlineStr">
+        <is>
+          <t>продам черепаху</t>
+        </is>
+      </c>
+      <c r="C34" s="0" t="inlineStr">
         <is>
           <t>19 июля 2022 г.</t>
         </is>
       </c>
-      <c r="D34" s="11" t="inlineStr">
+      <c r="D34" s="0" t="inlineStr">
         <is>
           <t>https://www.olx.kz/d/obyavlenie/prodam-motoekipirovku-cherepaha-IDm1Opx.html#fe43e5f20a</t>
         </is>
       </c>
-      <c r="E34" s="11" t="inlineStr">
+      <c r="E34" s="0" t="inlineStr">
         <is>
           <t>Мотоэкипировка остались шорты, наколенники и перчатки, в хорошем состоянии, размер XXL, ОДЕВАЛ НЕСКОЛЬКО РАЗ...</t>
         </is>
       </c>
     </row>
-    <row r="35" ht="41.75" customHeight="1" s="12">
-      <c r="A35" s="10" t="inlineStr">
+    <row r="35">
+      <c r="A35" s="0" t="inlineStr">
         <is>
           <t>34</t>
         </is>
       </c>
-      <c r="B35" s="11" t="inlineStr">
-        <is>
-          <t>продам черепаху</t>
-        </is>
-      </c>
-      <c r="C35" s="10" t="inlineStr">
+      <c r="B35" s="0" t="inlineStr">
+        <is>
+          <t>продам черепаху</t>
+        </is>
+      </c>
+      <c r="C35" s="0" t="inlineStr">
         <is>
           <t>19 июля 2022 г.</t>
         </is>
       </c>
-      <c r="D35" s="11" t="inlineStr">
+      <c r="D35" s="0" t="inlineStr">
         <is>
           <t>https://www.olx.kz/d/obyavlenie/prodam-monetu-iz-serebra-cherepaha-IDmmmH0.html#fe43e5f20a</t>
         </is>
       </c>
-      <c r="E35" s="11" t="inlineStr">
+      <c r="E35" s="0" t="inlineStr">
         <is>
           <t>Продам  монету  из серебра "Черепаха " в отличном состоянии, сертификат имеется.</t>
         </is>
       </c>
     </row>
-    <row r="36" ht="55.2" customHeight="1" s="12">
-      <c r="A36" s="10" t="inlineStr">
+    <row r="36">
+      <c r="A36" s="0" t="inlineStr">
         <is>
           <t>35</t>
         </is>
       </c>
-      <c r="B36" s="11" t="inlineStr">
-        <is>
-          <t>продам черепаху</t>
-        </is>
-      </c>
-      <c r="C36" s="10" t="inlineStr">
+      <c r="B36" s="0" t="inlineStr">
+        <is>
+          <t>продам черепаху</t>
+        </is>
+      </c>
+      <c r="C36" s="0" t="inlineStr">
         <is>
           <t>17 июля 2022 г.</t>
         </is>
       </c>
-      <c r="D36" s="11" t="inlineStr">
+      <c r="D36" s="0" t="inlineStr">
         <is>
           <t>https://www.olx.kz/d/obyavlenie/prodam-krasnouhuyu-cherepahuluchshego-pitomtsa-IDmGpl0.html#fe43e5f20a</t>
         </is>
       </c>
-      <c r="E36" s="11" t="inlineStr">
+      <c r="E36" s="0" t="inlineStr">
         <is>
           <t>Продаем красноухую черепаху. 
 Самого лучшего питомца.
@@ -1532,272 +1510,272 @@
         </is>
       </c>
     </row>
-    <row r="37" ht="28.35" customHeight="1" s="12">
-      <c r="A37" s="10" t="inlineStr">
+    <row r="37">
+      <c r="A37" s="0" t="inlineStr">
         <is>
           <t>36</t>
         </is>
       </c>
-      <c r="B37" s="11" t="inlineStr">
-        <is>
-          <t>продам черепаху</t>
-        </is>
-      </c>
-      <c r="C37" s="10" t="inlineStr">
+      <c r="B37" s="0" t="inlineStr">
+        <is>
+          <t>продам черепаху</t>
+        </is>
+      </c>
+      <c r="C37" s="0" t="inlineStr">
         <is>
           <t>16 июля 2022 г.</t>
         </is>
       </c>
-      <c r="D37" s="11" t="inlineStr">
+      <c r="D37" s="0" t="inlineStr">
         <is>
           <t>https://www.olx.kz/d/obyavlenie/prodam-cherepahu-ne-dorogo-IDmGlEg.html#fe43e5f20a</t>
         </is>
       </c>
-      <c r="E37" s="11" t="inlineStr">
+      <c r="E37" s="0" t="inlineStr">
         <is>
           <t>Продам черепаху за 10 т.тенге .. Обращаться по номеру 77077046678.     СРОЧНО ...</t>
         </is>
       </c>
     </row>
-    <row r="38" ht="41.75" customHeight="1" s="12">
-      <c r="A38" s="10" t="inlineStr">
+    <row r="38">
+      <c r="A38" s="0" t="inlineStr">
         <is>
           <t>37</t>
         </is>
       </c>
-      <c r="B38" s="11" t="inlineStr">
-        <is>
-          <t>продам черепаху</t>
-        </is>
-      </c>
-      <c r="C38" s="10" t="inlineStr">
+      <c r="B38" s="0" t="inlineStr">
+        <is>
+          <t>продам черепаху</t>
+        </is>
+      </c>
+      <c r="C38" s="0" t="inlineStr">
         <is>
           <t>16 июля 2022 г.</t>
         </is>
       </c>
-      <c r="D38" s="11" t="inlineStr">
+      <c r="D38" s="0" t="inlineStr">
         <is>
           <t>https://www.olx.kz/d/obyavlenie/prodam-novuyu-suvenirnuyu-cherepahu-iz-oae-za-5500-IDkSLyU.html#fe43e5f20a</t>
         </is>
       </c>
-      <c r="E38" s="11" t="inlineStr">
+      <c r="E38" s="0" t="inlineStr">
         <is>
           <t>Продам новую сувенирную черепаху из ОАЭ за 5500! Черепаха аккуратная и состоит из ракушек.</t>
         </is>
       </c>
     </row>
-    <row r="39" ht="41.75" customHeight="1" s="12">
-      <c r="A39" s="10" t="inlineStr">
+    <row r="39">
+      <c r="A39" s="0" t="inlineStr">
         <is>
           <t>38</t>
         </is>
       </c>
-      <c r="B39" s="11" t="inlineStr">
-        <is>
-          <t>продам черепаху</t>
-        </is>
-      </c>
-      <c r="C39" s="10" t="inlineStr">
+      <c r="B39" s="0" t="inlineStr">
+        <is>
+          <t>продам черепаху</t>
+        </is>
+      </c>
+      <c r="C39" s="0" t="inlineStr">
         <is>
           <t>16 июля 2022 г.</t>
         </is>
       </c>
-      <c r="D39" s="11" t="inlineStr">
+      <c r="D39" s="0" t="inlineStr">
         <is>
           <t>https://www.olx.kz/d/obyavlenie/prodam-cherepaha-trioniks-IDlqFQt.html#fe43e5f20a</t>
         </is>
       </c>
-      <c r="E39" s="11" t="inlineStr">
+      <c r="E39" s="0" t="inlineStr">
         <is>
           <t>Продам подростков мягкотелой черепахи - трионикс. Размер около 5см.отправка в регионы. Инстаграм:Аквариум актобе.</t>
         </is>
       </c>
     </row>
-    <row r="40" ht="28.35" customHeight="1" s="12">
-      <c r="A40" s="10" t="inlineStr">
+    <row r="40">
+      <c r="A40" s="0" t="inlineStr">
         <is>
           <t>39</t>
         </is>
       </c>
-      <c r="B40" s="11" t="inlineStr">
-        <is>
-          <t>продам черепаху</t>
-        </is>
-      </c>
-      <c r="C40" s="10" t="inlineStr">
+      <c r="B40" s="0" t="inlineStr">
+        <is>
+          <t>продам черепаху</t>
+        </is>
+      </c>
+      <c r="C40" s="0" t="inlineStr">
         <is>
           <t>16 июля 2022 г.</t>
         </is>
       </c>
-      <c r="D40" s="11" t="inlineStr">
+      <c r="D40" s="0" t="inlineStr">
         <is>
           <t>https://www.olx.kz/d/obyavlenie/prodam-suhoputnuyu-cherepahu-IDmGazZ.html#fe43e5f20a</t>
         </is>
       </c>
-      <c r="E40" s="11" t="inlineStr">
+      <c r="E40" s="0" t="inlineStr">
         <is>
           <t>Продам сухопутную среднию черепаху отличный вариант для подарка, с домиком и контенером, очень любит салат, огурцы, яблоко, морковь, клубнику, бананы и. т. д ватцап 87056061712</t>
         </is>
       </c>
     </row>
-    <row r="41" ht="28.35" customHeight="1" s="12">
-      <c r="A41" s="10" t="inlineStr">
+    <row r="41">
+      <c r="A41" s="0" t="inlineStr">
         <is>
           <t>40</t>
         </is>
       </c>
-      <c r="B41" s="11" t="inlineStr">
-        <is>
-          <t>продам черепаху</t>
-        </is>
-      </c>
-      <c r="C41" s="10" t="inlineStr">
+      <c r="B41" s="0" t="inlineStr">
+        <is>
+          <t>продам черепаху</t>
+        </is>
+      </c>
+      <c r="C41" s="0" t="inlineStr">
         <is>
           <t>16 июля 2022 г.</t>
         </is>
       </c>
-      <c r="D41" s="11" t="inlineStr">
+      <c r="D41" s="0" t="inlineStr">
         <is>
           <t>https://www.olx.kz/d/obyavlenie/prodam-suhoputnuyu-cherepahu-IDmG9Mb.html#fe43e5f20a</t>
         </is>
       </c>
-      <c r="E41" s="11" t="inlineStr">
+      <c r="E41" s="0" t="inlineStr">
         <is>
           <t>Продам сухопутную черепаху молодая
 Все вопросы по телефону либо ват сап 87056699417</t>
         </is>
       </c>
     </row>
-    <row r="42" ht="202.95" customHeight="1" s="12">
-      <c r="A42" s="10" t="inlineStr">
+    <row r="42">
+      <c r="A42" s="0" t="inlineStr">
         <is>
           <t>41</t>
         </is>
       </c>
-      <c r="B42" s="11" t="inlineStr">
-        <is>
-          <t>продам черепаху</t>
-        </is>
-      </c>
-      <c r="C42" s="10" t="inlineStr">
+      <c r="B42" s="0" t="inlineStr">
+        <is>
+          <t>продам черепаху</t>
+        </is>
+      </c>
+      <c r="C42" s="0" t="inlineStr">
         <is>
           <t>16 июля 2022 г.</t>
         </is>
       </c>
-      <c r="D42" s="11" t="inlineStr">
+      <c r="D42" s="0" t="inlineStr">
         <is>
           <t>https://www.olx.kz/d/obyavlenie/prodam-suhoputnuyu-cherepahu-IDmG9dL.html#fe43e5f20a</t>
         </is>
       </c>
-      <c r="E42" s="11" t="inlineStr">
+      <c r="E42" s="0" t="inlineStr">
         <is>
           <t>Продам сухопутную черепаху, очень активная, неприхотливое животное, питается растительностью, будет отличным подарком для ваших деток</t>
         </is>
       </c>
     </row>
-    <row r="43" ht="41.75" customHeight="1" s="12">
-      <c r="A43" s="10" t="inlineStr">
+    <row r="43">
+      <c r="A43" s="0" t="inlineStr">
         <is>
           <t>42</t>
         </is>
       </c>
-      <c r="B43" s="11" t="inlineStr">
-        <is>
-          <t>продам черепаху</t>
-        </is>
-      </c>
-      <c r="C43" s="10" t="inlineStr">
+      <c r="B43" s="0" t="inlineStr">
+        <is>
+          <t>продам черепаху</t>
+        </is>
+      </c>
+      <c r="C43" s="0" t="inlineStr">
         <is>
           <t>15 июля 2022 г.</t>
         </is>
       </c>
-      <c r="D43" s="11" t="inlineStr">
+      <c r="D43" s="0" t="inlineStr">
         <is>
           <t>https://www.olx.kz/d/obyavlenie/srochno-prodam-cherepahu-scoyco-razmer-l-IDlZ3jj.html#fe43e5f20a</t>
         </is>
       </c>
-      <c r="E43" s="11" t="inlineStr">
+      <c r="E43" s="0" t="inlineStr">
         <is>
           <t>Срочно продам черепаху scoyco размер L одевался пару раз  брал в автопилоте  за 60 000 имеется небольшой торг</t>
         </is>
       </c>
     </row>
-    <row r="44" ht="68.65000000000001" customHeight="1" s="12">
-      <c r="A44" s="10" t="inlineStr">
+    <row r="44">
+      <c r="A44" s="0" t="inlineStr">
         <is>
           <t>43</t>
         </is>
       </c>
-      <c r="B44" s="11" t="inlineStr">
-        <is>
-          <t>продам черепаху</t>
-        </is>
-      </c>
-      <c r="C44" s="10" t="inlineStr">
+      <c r="B44" s="0" t="inlineStr">
+        <is>
+          <t>продам черепаху</t>
+        </is>
+      </c>
+      <c r="C44" s="0" t="inlineStr">
         <is>
           <t>15 июля 2022 г.</t>
         </is>
       </c>
-      <c r="D44" s="11" t="inlineStr">
+      <c r="D44" s="0" t="inlineStr">
         <is>
           <t>https://www.olx.kz/d/obyavlenie/prodam-suhoputnuyu-cherepahu-IDmFZ2a.html#fe43e5f20a</t>
         </is>
       </c>
-      <c r="E44" s="11" t="inlineStr">
+      <c r="E44" s="0" t="inlineStr">
         <is>
           <t>Продам сухопутную черепаху. Забавный и только в хорошие,добрые руки. Цена 5000 тг.</t>
         </is>
       </c>
     </row>
-    <row r="45" ht="28.35" customHeight="1" s="12">
-      <c r="A45" s="10" t="inlineStr">
+    <row r="45">
+      <c r="A45" s="0" t="inlineStr">
         <is>
           <t>44</t>
         </is>
       </c>
-      <c r="B45" s="11" t="inlineStr">
-        <is>
-          <t>продам черепаху</t>
-        </is>
-      </c>
-      <c r="C45" s="10" t="inlineStr">
+      <c r="B45" s="0" t="inlineStr">
+        <is>
+          <t>продам черепаху</t>
+        </is>
+      </c>
+      <c r="C45" s="0" t="inlineStr">
         <is>
           <t>15 июля 2022 г.</t>
         </is>
       </c>
-      <c r="D45" s="11" t="inlineStr">
+      <c r="D45" s="0" t="inlineStr">
         <is>
           <t>https://www.olx.kz/d/obyavlenie/prodam-akvarium-dlya-cherepahi-IDmvWE2.html#fe43e5f20a</t>
         </is>
       </c>
-      <c r="E45" s="11" t="inlineStr">
+      <c r="E45" s="0" t="inlineStr">
         <is>
           <t>Продам аквариум для черепахи. В хорошем состоянии</t>
         </is>
       </c>
     </row>
-    <row r="46" ht="28.35" customHeight="1" s="12">
-      <c r="A46" s="10" t="inlineStr">
+    <row r="46">
+      <c r="A46" s="0" t="inlineStr">
         <is>
           <t>45</t>
         </is>
       </c>
-      <c r="B46" s="11" t="inlineStr">
-        <is>
-          <t>продам черепаху</t>
-        </is>
-      </c>
-      <c r="C46" s="10" t="inlineStr">
+      <c r="B46" s="0" t="inlineStr">
+        <is>
+          <t>продам черепаху</t>
+        </is>
+      </c>
+      <c r="C46" s="0" t="inlineStr">
         <is>
           <t>14 июля 2022 г.</t>
         </is>
       </c>
-      <c r="D46" s="11" t="inlineStr">
+      <c r="D46" s="0" t="inlineStr">
         <is>
           <t>https://www.olx.kz/d/obyavlenie/prodam-suhoputnuyu-cherepahu-IDmbEy6.html#fe43e5f20a</t>
         </is>
       </c>
-      <c r="E46" s="11" t="inlineStr">
+      <c r="E46" s="0" t="inlineStr">
         <is>
           <t>Каждый из нас хоть однажды оказывался перед непростой дилеммой: заводить или нет домашнее животное. А если да, то — какое? Собаку, кошку, кролика или попугая? Принять решение непросто, ведь питомец потребует дополнительных расходов, внимания и ухода. Если вы переживаете, что не сможете уделять ему достаточно времени, боитесь, что животное окажется назойливым, вам стоит завести сухопутную черепаху.
 Черепахи неприхотливые животные, у них хороший характер. Они не опасны для детей.
@@ -1806,218 +1784,218 @@
         </is>
       </c>
     </row>
-    <row r="47" ht="41.75" customHeight="1" s="12">
-      <c r="A47" s="10" t="inlineStr">
+    <row r="47">
+      <c r="A47" s="0" t="inlineStr">
         <is>
           <t>46</t>
         </is>
       </c>
-      <c r="B47" s="11" t="inlineStr">
-        <is>
-          <t>продам черепаху</t>
-        </is>
-      </c>
-      <c r="C47" s="10" t="inlineStr">
+      <c r="B47" s="0" t="inlineStr">
+        <is>
+          <t>продам черепаху</t>
+        </is>
+      </c>
+      <c r="C47" s="0" t="inlineStr">
         <is>
           <t>14 июля 2022 г.</t>
         </is>
       </c>
-      <c r="D47" s="11" t="inlineStr">
+      <c r="D47" s="0" t="inlineStr">
         <is>
           <t>https://www.olx.kz/d/obyavlenie/cherepaha-prodam-cherepahu-IDmacNw.html#fe43e5f20a</t>
         </is>
       </c>
-      <c r="E47" s="11" t="inlineStr">
+      <c r="E47" s="0" t="inlineStr">
         <is>
           <t>Продам черепах. Большая 3000тг
 Средняя 4000тг. В еде не прихотливы. Едят траву, овощи, фрукты</t>
         </is>
       </c>
     </row>
-    <row r="48" ht="41.75" customHeight="1" s="12">
-      <c r="A48" s="10" t="inlineStr">
+    <row r="48">
+      <c r="A48" s="0" t="inlineStr">
         <is>
           <t>47</t>
         </is>
       </c>
-      <c r="B48" s="11" t="inlineStr">
-        <is>
-          <t>продам черепаху</t>
-        </is>
-      </c>
-      <c r="C48" s="10" t="inlineStr">
+      <c r="B48" s="0" t="inlineStr">
+        <is>
+          <t>продам черепаху</t>
+        </is>
+      </c>
+      <c r="C48" s="0" t="inlineStr">
         <is>
           <t>14 июля 2022 г.</t>
         </is>
       </c>
-      <c r="D48" s="11" t="inlineStr">
+      <c r="D48" s="0" t="inlineStr">
         <is>
           <t>https://www.olx.kz/d/obyavlenie/prodam-morskuyu-krasnouhuyu-cherepahu-IDlE7tK.html#fe43e5f20a</t>
         </is>
       </c>
-      <c r="E48" s="11" t="inlineStr">
+      <c r="E48" s="0" t="inlineStr">
         <is>
           <t>Продам морскую черепаху. Маленькая, живет в аквариуме, питается спец замороженным кормом. Вообще неприхотливая. Отличный питомец,  не требующий больших затрат времени и денег на уход и содержание. Цена без аквариума.</t>
         </is>
       </c>
     </row>
-    <row r="49" ht="41.75" customHeight="1" s="12">
-      <c r="A49" s="10" t="inlineStr">
+    <row r="49">
+      <c r="A49" s="0" t="inlineStr">
         <is>
           <t>48</t>
         </is>
       </c>
-      <c r="B49" s="11" t="inlineStr">
-        <is>
-          <t>продам черепаху</t>
-        </is>
-      </c>
-      <c r="C49" s="10" t="inlineStr">
+      <c r="B49" s="0" t="inlineStr">
+        <is>
+          <t>продам черепаху</t>
+        </is>
+      </c>
+      <c r="C49" s="0" t="inlineStr">
         <is>
           <t>13 июля 2022 г.</t>
         </is>
       </c>
-      <c r="D49" s="11" t="inlineStr">
+      <c r="D49" s="0" t="inlineStr">
         <is>
           <t>https://www.olx.kz/d/obyavlenie/prodam-cherepahu-IDmFARG.html#fe43e5f20a</t>
         </is>
       </c>
-      <c r="E49" s="11" t="inlineStr">
+      <c r="E49" s="0" t="inlineStr">
         <is>
           <t>Продам красноухую черепаху вместе с  аквариумом,питается мотылем за 15000</t>
         </is>
       </c>
     </row>
-    <row r="50" ht="95.5" customHeight="1" s="12">
-      <c r="A50" s="10" t="inlineStr">
+    <row r="50">
+      <c r="A50" s="0" t="inlineStr">
         <is>
           <t>49</t>
         </is>
       </c>
-      <c r="B50" s="11" t="inlineStr">
-        <is>
-          <t>продам черепаху</t>
-        </is>
-      </c>
-      <c r="C50" s="10" t="inlineStr">
+      <c r="B50" s="0" t="inlineStr">
+        <is>
+          <t>продам черепаху</t>
+        </is>
+      </c>
+      <c r="C50" s="0" t="inlineStr">
         <is>
           <t>13 июля 2022 г.</t>
         </is>
       </c>
-      <c r="D50" s="11" t="inlineStr">
+      <c r="D50" s="0" t="inlineStr">
         <is>
           <t>https://www.olx.kz/d/obyavlenie/prodam-krasnouhuyu-cherepahu-IDmwWxF.html#fe43e5f20a</t>
         </is>
       </c>
-      <c r="E50" s="11" t="inlineStr">
+      <c r="E50" s="0" t="inlineStr">
         <is>
           <t>Продам красноухую черепаху с аквариумом, фильтром и домиком. Вопросы по телефону</t>
         </is>
       </c>
     </row>
-    <row r="51" ht="68.65000000000001" customHeight="1" s="12">
-      <c r="A51" s="10" t="inlineStr">
+    <row r="51">
+      <c r="A51" s="0" t="inlineStr">
         <is>
           <t>50</t>
         </is>
       </c>
-      <c r="B51" s="11" t="inlineStr">
-        <is>
-          <t>продам черепаху</t>
-        </is>
-      </c>
-      <c r="C51" s="10" t="inlineStr">
+      <c r="B51" s="0" t="inlineStr">
+        <is>
+          <t>продам черепаху</t>
+        </is>
+      </c>
+      <c r="C51" s="0" t="inlineStr">
         <is>
           <t>12 июля 2022 г.</t>
         </is>
       </c>
-      <c r="D51" s="11" t="inlineStr">
+      <c r="D51" s="0" t="inlineStr">
         <is>
           <t>https://www.olx.kz/d/obyavlenie/prodam-terrarium-vmeste-s-krasnouhoy-cherepahoy-55tys-tenge-IDlxTaB.html#fe43e5f20a</t>
         </is>
       </c>
-      <c r="E51" s="11" t="inlineStr">
+      <c r="E51" s="0" t="inlineStr">
         <is>
           <t>Отличный подарок вашим деткам к новому году.терариум объем воды 120 литров. Прочное стекло.</t>
         </is>
       </c>
     </row>
-    <row r="52" ht="122.35" customHeight="1" s="12">
-      <c r="A52" s="10" t="inlineStr">
+    <row r="52">
+      <c r="A52" s="0" t="inlineStr">
         <is>
           <t>51</t>
         </is>
       </c>
-      <c r="B52" s="11" t="inlineStr">
-        <is>
-          <t>продам черепаху</t>
-        </is>
-      </c>
-      <c r="C52" s="10" t="inlineStr">
+      <c r="B52" s="0" t="inlineStr">
+        <is>
+          <t>продам черепаху</t>
+        </is>
+      </c>
+      <c r="C52" s="0" t="inlineStr">
         <is>
           <t>11 июля 2022 г.</t>
         </is>
       </c>
-      <c r="D52" s="11" t="inlineStr">
+      <c r="D52" s="0" t="inlineStr">
         <is>
           <t>https://www.olx.kz/d/obyavlenie/prodam-2-cherepahi-IDlRXt8.html#fe43e5f20a</t>
         </is>
       </c>
-      <c r="E52" s="11" t="inlineStr">
+      <c r="E52" s="0" t="inlineStr">
         <is>
           <t>Продам две черепахи имеется всё необходимое, аквариум 10 тыс.тг очист с Вит, корм и все принадлежности</t>
         </is>
       </c>
     </row>
-    <row r="53" ht="28.35" customHeight="1" s="12">
-      <c r="A53" s="10" t="inlineStr">
+    <row r="53">
+      <c r="A53" s="0" t="inlineStr">
         <is>
           <t>52</t>
         </is>
       </c>
-      <c r="B53" s="11" t="inlineStr">
-        <is>
-          <t>продам черепаху</t>
-        </is>
-      </c>
-      <c r="C53" s="10" t="inlineStr">
+      <c r="B53" s="0" t="inlineStr">
+        <is>
+          <t>продам черепаху</t>
+        </is>
+      </c>
+      <c r="C53" s="0" t="inlineStr">
         <is>
           <t>11 июля 2022 г.</t>
         </is>
       </c>
-      <c r="D53" s="11" t="inlineStr">
+      <c r="D53" s="0" t="inlineStr">
         <is>
           <t>https://www.olx.kz/d/obyavlenie/prodam-cherepahu-razmery-primerno-15-519-santimetrov-IDme0qa.html#fe43e5f20a</t>
         </is>
       </c>
-      <c r="E53" s="11" t="inlineStr">
+      <c r="E53" s="0" t="inlineStr">
         <is>
           <t>Черепаха . сухопутная</t>
         </is>
       </c>
     </row>
-    <row r="54" ht="41.75" customHeight="1" s="12">
-      <c r="A54" s="10" t="inlineStr">
+    <row r="54">
+      <c r="A54" s="0" t="inlineStr">
         <is>
           <t>53</t>
         </is>
       </c>
-      <c r="B54" s="11" t="inlineStr">
-        <is>
-          <t>продам черепаху</t>
-        </is>
-      </c>
-      <c r="C54" s="10" t="inlineStr">
+      <c r="B54" s="0" t="inlineStr">
+        <is>
+          <t>продам черепаху</t>
+        </is>
+      </c>
+      <c r="C54" s="0" t="inlineStr">
         <is>
           <t>09 июля 2022 г.</t>
         </is>
       </c>
-      <c r="D54" s="11" t="inlineStr">
+      <c r="D54" s="0" t="inlineStr">
         <is>
           <t>https://www.olx.kz/d/obyavlenie/prodam-cherepaha-krasnouhaya-IDmuy1F.html#fe43e5f20a</t>
         </is>
       </c>
-      <c r="E54" s="11" t="inlineStr">
+      <c r="E54" s="0" t="inlineStr">
         <is>
           <t>Красноухая черепаха, молодая - 2 года (продолжительность жизни при должном уходе 40-50 лет). Пресноводная - необходим аквариум. Размер 15-20см. 
  аквариум 10000тг 60 литров
@@ -2026,353 +2004,353 @@
         </is>
       </c>
     </row>
-    <row r="55" ht="28.35" customHeight="1" s="12">
-      <c r="A55" s="10" t="inlineStr">
+    <row r="55">
+      <c r="A55" s="0" t="inlineStr">
         <is>
           <t>54</t>
         </is>
       </c>
-      <c r="B55" s="11" t="inlineStr">
-        <is>
-          <t>продам черепаху</t>
-        </is>
-      </c>
-      <c r="C55" s="10" t="inlineStr">
+      <c r="B55" s="0" t="inlineStr">
+        <is>
+          <t>продам черепаху</t>
+        </is>
+      </c>
+      <c r="C55" s="0" t="inlineStr">
         <is>
           <t>08 июля 2022 г.</t>
         </is>
       </c>
-      <c r="D55" s="11" t="inlineStr">
+      <c r="D55" s="0" t="inlineStr">
         <is>
           <t>https://www.olx.kz/d/obyavlenie/prodam-suhoputnuyu-cherepahu-IDmE6T6.html#fe43e5f20a</t>
         </is>
       </c>
-      <c r="E55" s="11" t="inlineStr">
+      <c r="E55" s="0" t="inlineStr">
         <is>
           <t>Продам сухопутную черепаху , девочка, зовут Бонни, питается клевером , одуванчиком и может даже сеном , дополнительной пищей могут являться овощи и фрукты. Черепаха не прихотливое животное , и всегда будет интересна вам и вашим детям!</t>
         </is>
       </c>
     </row>
-    <row r="56" ht="41.75" customHeight="1" s="12">
-      <c r="A56" s="10" t="inlineStr">
+    <row r="56">
+      <c r="A56" s="0" t="inlineStr">
         <is>
           <t>55</t>
         </is>
       </c>
-      <c r="B56" s="11" t="inlineStr">
-        <is>
-          <t>продам черепаху</t>
-        </is>
-      </c>
-      <c r="C56" s="10" t="inlineStr">
+      <c r="B56" s="0" t="inlineStr">
+        <is>
+          <t>продам черепаху</t>
+        </is>
+      </c>
+      <c r="C56" s="0" t="inlineStr">
         <is>
           <t>08 июля 2022 г.</t>
         </is>
       </c>
-      <c r="D56" s="11" t="inlineStr">
+      <c r="D56" s="0" t="inlineStr">
         <is>
           <t>https://www.olx.kz/d/obyavlenie/prodam-cherepahu-5000-IDmDRG4.html#fe43e5f20a</t>
         </is>
       </c>
-      <c r="E56" s="11" t="inlineStr">
+      <c r="E56" s="0" t="inlineStr">
         <is>
           <t>Продам черепаху 5000
 Черепахи относятся к классу пресмыкающихся или рептилий. На нашей планете их существует около 340 форм, которые делятся на морские и наземные. Наземные черепахи, в свою очередь, подразделяются на сухопутные и пресноводные. Появились эти рептилии более 200 миллионов лет назад, в эпоху динозавров.</t>
         </is>
       </c>
     </row>
-    <row r="57" ht="28.35" customHeight="1" s="12">
-      <c r="A57" s="10" t="inlineStr">
+    <row r="57">
+      <c r="A57" s="0" t="inlineStr">
         <is>
           <t>56</t>
         </is>
       </c>
-      <c r="B57" s="11" t="inlineStr">
-        <is>
-          <t>продам черепаху</t>
-        </is>
-      </c>
-      <c r="C57" s="10" t="inlineStr">
+      <c r="B57" s="0" t="inlineStr">
+        <is>
+          <t>продам черепаху</t>
+        </is>
+      </c>
+      <c r="C57" s="0" t="inlineStr">
         <is>
           <t>07 июля 2022 г.</t>
         </is>
       </c>
-      <c r="D57" s="11" t="inlineStr">
+      <c r="D57" s="0" t="inlineStr">
         <is>
           <t>https://www.olx.kz/d/obyavlenie/akvarium-prodam-dlya-cherepahi-IDmuipb.html#fe43e5f20a</t>
         </is>
       </c>
-      <c r="E57" s="11" t="inlineStr">
+      <c r="E57" s="0" t="inlineStr">
         <is>
           <t>Продам аквариум для черепашки или можно для хомяка. Писать на ватсап 87081521874</t>
         </is>
       </c>
     </row>
-    <row r="58" ht="28.35" customHeight="1" s="12">
-      <c r="A58" s="10" t="inlineStr">
+    <row r="58">
+      <c r="A58" s="0" t="inlineStr">
         <is>
           <t>57</t>
         </is>
       </c>
-      <c r="B58" s="11" t="inlineStr">
-        <is>
-          <t>продам черепаху</t>
-        </is>
-      </c>
-      <c r="C58" s="10" t="inlineStr">
+      <c r="B58" s="0" t="inlineStr">
+        <is>
+          <t>продам черепаху</t>
+        </is>
+      </c>
+      <c r="C58" s="0" t="inlineStr">
         <is>
           <t>07 июля 2022 г.</t>
         </is>
       </c>
-      <c r="D58" s="11" t="inlineStr">
+      <c r="D58" s="0" t="inlineStr">
         <is>
           <t>https://www.olx.kz/d/obyavlenie/prodam-filtr-dlya-cherepahi-IDkb3wg.html#fe43e5f20a</t>
         </is>
       </c>
-      <c r="E58" s="11" t="inlineStr">
+      <c r="E58" s="0" t="inlineStr">
         <is>
           <t>Продам фильтр для очистки воды,островок для черепах,пользовались месяц по этой же цене,что и брали,7000т</t>
         </is>
       </c>
     </row>
-    <row r="59" ht="28.35" customHeight="1" s="12">
-      <c r="A59" s="10" t="inlineStr">
+    <row r="59">
+      <c r="A59" s="0" t="inlineStr">
         <is>
           <t>58</t>
         </is>
       </c>
-      <c r="B59" s="11" t="inlineStr">
-        <is>
-          <t>продам черепаху</t>
-        </is>
-      </c>
-      <c r="C59" s="10" t="inlineStr">
+      <c r="B59" s="0" t="inlineStr">
+        <is>
+          <t>продам черепаху</t>
+        </is>
+      </c>
+      <c r="C59" s="0" t="inlineStr">
         <is>
           <t>07 июля 2022 г.</t>
         </is>
       </c>
-      <c r="D59" s="11" t="inlineStr">
+      <c r="D59" s="0" t="inlineStr">
         <is>
           <t>https://www.olx.kz/d/obyavlenie/prodam-cherepahu-s-akvariumom-IDmDLBt.html#fe43e5f20a</t>
         </is>
       </c>
-      <c r="E59" s="11" t="inlineStr">
+      <c r="E59" s="0" t="inlineStr">
         <is>
           <t>Продам черепаху девочку взрослая вместе с аквариумом и наполнителем звоните пишите</t>
         </is>
       </c>
     </row>
-    <row r="60" ht="41.75" customHeight="1" s="12">
-      <c r="A60" s="10" t="inlineStr">
+    <row r="60">
+      <c r="A60" s="0" t="inlineStr">
         <is>
           <t>59</t>
         </is>
       </c>
-      <c r="B60" s="11" t="inlineStr">
-        <is>
-          <t>продам черепаху</t>
-        </is>
-      </c>
-      <c r="C60" s="10" t="inlineStr">
+      <c r="B60" s="0" t="inlineStr">
+        <is>
+          <t>продам черепаху</t>
+        </is>
+      </c>
+      <c r="C60" s="0" t="inlineStr">
         <is>
           <t>07 июля 2022 г.</t>
         </is>
       </c>
-      <c r="D60" s="11" t="inlineStr">
-        <is>
-          <t>https://www.olx.kz/d/obyavlenie/prodam-krasnouhuyu-cherepahu-IDmDzYS.html#fe43e5f20a</t>
-        </is>
-      </c>
-      <c r="E60" s="11" t="inlineStr">
+      <c r="D60" s="0" t="inlineStr">
+        <is>
+          <t>https://www.olx.kz/d/obyavlenie/prodam-krasnouhuyu-cherepahu-IDmDzYS.html#729a76a98a</t>
+        </is>
+      </c>
+      <c r="E60" s="0" t="inlineStr">
         <is>
           <t>Продам черепаху красноухую аквариума нет сломался девочка корм можете купить зоомагазине</t>
         </is>
       </c>
     </row>
-    <row r="61" ht="28.35" customHeight="1" s="12">
-      <c r="A61" s="10" t="inlineStr">
+    <row r="61">
+      <c r="A61" s="0" t="inlineStr">
         <is>
           <t>60</t>
         </is>
       </c>
-      <c r="B61" s="11" t="inlineStr">
-        <is>
-          <t>продам черепаху</t>
-        </is>
-      </c>
-      <c r="C61" s="10" t="inlineStr">
+      <c r="B61" s="0" t="inlineStr">
+        <is>
+          <t>продам черепаху</t>
+        </is>
+      </c>
+      <c r="C61" s="0" t="inlineStr">
         <is>
           <t>06 июля 2022 г.</t>
         </is>
       </c>
-      <c r="D61" s="11" t="inlineStr">
-        <is>
-          <t>https://www.olx.kz/d/obyavlenie/prodam-cherepahu-IDmDp14.html#fe43e5f20a</t>
-        </is>
-      </c>
-      <c r="E61" s="11" t="inlineStr">
+      <c r="D61" s="0" t="inlineStr">
+        <is>
+          <t>https://www.olx.kz/d/obyavlenie/prodam-cherepahu-IDmDp14.html#729a76a98a</t>
+        </is>
+      </c>
+      <c r="E61" s="0" t="inlineStr">
         <is>
           <t>Продаётся черепаха! Двое за 8 тысяч. Один стоит 4 тысячи. Звоните по номеру 87775658664</t>
         </is>
       </c>
     </row>
-    <row r="62" ht="55.2" customHeight="1" s="12">
-      <c r="A62" s="10" t="inlineStr">
+    <row r="62">
+      <c r="A62" s="0" t="inlineStr">
         <is>
           <t>61</t>
         </is>
       </c>
-      <c r="B62" s="11" t="inlineStr">
-        <is>
-          <t>продам черепаху</t>
-        </is>
-      </c>
-      <c r="C62" s="10" t="inlineStr">
+      <c r="B62" s="0" t="inlineStr">
+        <is>
+          <t>продам черепаху</t>
+        </is>
+      </c>
+      <c r="C62" s="0" t="inlineStr">
         <is>
           <t>06 июля 2022 г.</t>
         </is>
       </c>
-      <c r="D62" s="11" t="inlineStr">
+      <c r="D62" s="0" t="inlineStr">
         <is>
           <t>https://www.olx.kz/d/obyavlenie/prodam-cherepahu-i-begemota-IDkxEOg.html#729a76a98a</t>
         </is>
       </c>
-      <c r="E62" s="11" t="inlineStr">
+      <c r="E62" s="0" t="inlineStr">
         <is>
           <t>Продам   подушки     в   виде   зверюшек.   Бегемот     1000.   Черепаха     1500</t>
         </is>
       </c>
     </row>
-    <row r="63" ht="28.35" customHeight="1" s="12">
-      <c r="A63" s="10" t="inlineStr">
+    <row r="63">
+      <c r="A63" s="0" t="inlineStr">
         <is>
           <t>62</t>
         </is>
       </c>
-      <c r="B63" s="11" t="inlineStr">
-        <is>
-          <t>продам черепаху</t>
-        </is>
-      </c>
-      <c r="C63" s="10" t="inlineStr">
+      <c r="B63" s="0" t="inlineStr">
+        <is>
+          <t>продам черепаху</t>
+        </is>
+      </c>
+      <c r="C63" s="0" t="inlineStr">
         <is>
           <t>06 июля 2022 г.</t>
         </is>
       </c>
-      <c r="D63" s="11" t="inlineStr">
+      <c r="D63" s="0" t="inlineStr">
         <is>
           <t>https://www.olx.kz/d/obyavlenie/prodam-moto-perchatki-kurtka-zaschita-nog-cherepaha-sumka-na-poyas-IDkMSuG.html#729a76a98a</t>
         </is>
       </c>
-      <c r="E63" s="11" t="inlineStr">
+      <c r="E63" s="0" t="inlineStr">
         <is>
           <t>перчатки,балаклава,сумка на пояс,сумка которая крепится на Мот(с магнитами),куртка,защита ног,черепаха,подномерник</t>
         </is>
       </c>
     </row>
-    <row r="64" ht="82.05" customHeight="1" s="12">
-      <c r="A64" s="10" t="inlineStr">
+    <row r="64">
+      <c r="A64" s="0" t="inlineStr">
         <is>
           <t>63</t>
         </is>
       </c>
-      <c r="B64" s="11" t="inlineStr">
-        <is>
-          <t>продам черепаху</t>
-        </is>
-      </c>
-      <c r="C64" s="10" t="inlineStr">
+      <c r="B64" s="0" t="inlineStr">
+        <is>
+          <t>продам черепаху</t>
+        </is>
+      </c>
+      <c r="C64" s="0" t="inlineStr">
         <is>
           <t>05 июля 2022 г.</t>
         </is>
       </c>
-      <c r="D64" s="11" t="inlineStr">
+      <c r="D64" s="0" t="inlineStr">
         <is>
           <t>https://www.olx.kz/d/obyavlenie/prodam-cherepahu-obychnaya-suhoputnaya-IDmD70f.html#729a76a98a</t>
         </is>
       </c>
-      <c r="E64" s="11" t="inlineStr">
+      <c r="E64" s="0" t="inlineStr">
         <is>
           <t>Продам черепаху, обычную, сухопутную, 5000 тенге</t>
         </is>
       </c>
     </row>
-    <row r="65" ht="55.2" customHeight="1" s="12">
-      <c r="A65" s="10" t="inlineStr">
+    <row r="65">
+      <c r="A65" s="0" t="inlineStr">
         <is>
           <t>64</t>
         </is>
       </c>
-      <c r="B65" s="11" t="inlineStr">
-        <is>
-          <t>продам черепаху</t>
-        </is>
-      </c>
-      <c r="C65" s="10" t="inlineStr">
+      <c r="B65" s="0" t="inlineStr">
+        <is>
+          <t>продам черепаху</t>
+        </is>
+      </c>
+      <c r="C65" s="0" t="inlineStr">
         <is>
           <t>05 июля 2022 г.</t>
         </is>
       </c>
-      <c r="D65" s="11" t="inlineStr">
+      <c r="D65" s="0" t="inlineStr">
         <is>
           <t>https://www.olx.kz/d/obyavlenie/prodam-nochnik-cherepaha-IDmCQ7j.html#729a76a98a</t>
         </is>
       </c>
-      <c r="E65" s="11" t="inlineStr">
+      <c r="E65" s="0" t="inlineStr">
         <is>
           <t>Продам ночник черепаха работает хорошо светит разными цветами, поможет ребёнку уснуть без света в комнате.торга нет смотреть на Саина домостроительной</t>
         </is>
       </c>
     </row>
-    <row r="66" ht="28.35" customHeight="1" s="12">
-      <c r="A66" s="10" t="inlineStr">
+    <row r="66">
+      <c r="A66" s="0" t="inlineStr">
         <is>
           <t>65</t>
         </is>
       </c>
-      <c r="B66" s="11" t="inlineStr">
-        <is>
-          <t>продам черепаху</t>
-        </is>
-      </c>
-      <c r="C66" s="10" t="inlineStr">
+      <c r="B66" s="0" t="inlineStr">
+        <is>
+          <t>продам черепаху</t>
+        </is>
+      </c>
+      <c r="C66" s="0" t="inlineStr">
         <is>
           <t>05 июля 2022 г.</t>
         </is>
       </c>
-      <c r="D66" s="11" t="inlineStr">
+      <c r="D66" s="0" t="inlineStr">
         <is>
           <t>https://www.olx.kz/d/obyavlenie/prodam-detskiy-kovrik-cherepaha-srochno-IDkX4uK.html#729a76a98a</t>
         </is>
       </c>
-      <c r="E66" s="11" t="inlineStr">
+      <c r="E66" s="0" t="inlineStr">
         <is>
           <t>Пррдам срочно коврик черепаха зеленого цвета в  хорошем состоянии, чистый. Самовывоз. Каскелен.</t>
         </is>
       </c>
     </row>
-    <row r="67" ht="28.35" customHeight="1" s="12">
-      <c r="A67" s="10" t="inlineStr">
+    <row r="67">
+      <c r="A67" s="0" t="inlineStr">
         <is>
           <t>66</t>
         </is>
       </c>
-      <c r="B67" s="11" t="inlineStr">
-        <is>
-          <t>продам черепаху</t>
-        </is>
-      </c>
-      <c r="C67" s="10" t="inlineStr">
+      <c r="B67" s="0" t="inlineStr">
+        <is>
+          <t>продам черепаху</t>
+        </is>
+      </c>
+      <c r="C67" s="0" t="inlineStr">
         <is>
           <t>04 июля 2022 г.</t>
         </is>
       </c>
-      <c r="D67" s="11" t="inlineStr">
+      <c r="D67" s="0" t="inlineStr">
         <is>
           <t>https://www.olx.kz/d/obyavlenie/prodam-cherepahu-razmer-xl-IDmCNlP.html#729a76a98a</t>
         </is>
       </c>
-      <c r="E67" s="11" t="inlineStr">
+      <c r="E67" s="0" t="inlineStr">
         <is>
           <t>Продам   
 Черепаху
@@ -2383,28 +2361,28 @@
         </is>
       </c>
     </row>
-    <row r="68" ht="28.35" customHeight="1" s="12">
-      <c r="A68" s="10" t="inlineStr">
+    <row r="68">
+      <c r="A68" s="0" t="inlineStr">
         <is>
           <t>67</t>
         </is>
       </c>
-      <c r="B68" s="18" t="inlineStr">
-        <is>
-          <t>продам черепаху</t>
-        </is>
-      </c>
-      <c r="C68" s="19" t="inlineStr">
+      <c r="B68" s="0" t="inlineStr">
+        <is>
+          <t>продам черепаху</t>
+        </is>
+      </c>
+      <c r="C68" s="0" t="inlineStr">
         <is>
           <t>04 июля 2022 г.</t>
         </is>
       </c>
-      <c r="D68" s="18" t="inlineStr">
+      <c r="D68" s="0" t="inlineStr">
         <is>
           <t>https://www.olx.kz/d/obyavlenie/prodam-suhoputnuyu-cherepahu-IDmCHdc.html#729a76a98a</t>
         </is>
       </c>
-      <c r="E68" s="18" t="inlineStr">
+      <c r="E68" s="0" t="inlineStr">
         <is>
           <t>черепашке 8лет, добрая, спокойная, неконфликтная, не кусается. 
 ест только салат и кабачки. 
@@ -2412,82 +2390,82 @@
         </is>
       </c>
     </row>
-    <row r="69" ht="28.35" customHeight="1" s="12">
-      <c r="A69" s="10" t="inlineStr">
+    <row r="69">
+      <c r="A69" s="0" t="inlineStr">
         <is>
           <t>68</t>
         </is>
       </c>
-      <c r="B69" s="11" t="inlineStr">
-        <is>
-          <t>продам черепаху</t>
-        </is>
-      </c>
-      <c r="C69" s="10" t="inlineStr">
+      <c r="B69" s="0" t="inlineStr">
+        <is>
+          <t>продам черепаху</t>
+        </is>
+      </c>
+      <c r="C69" s="0" t="inlineStr">
         <is>
           <t>04 июля 2022 г.</t>
         </is>
       </c>
-      <c r="D69" s="11" t="inlineStr">
+      <c r="D69" s="0" t="inlineStr">
         <is>
           <t>https://www.olx.kz/d/obyavlenie/prodam-krasnouhaya-cherepaha-IDl06KK.html#729a76a98a</t>
         </is>
       </c>
-      <c r="E69" s="11" t="inlineStr">
+      <c r="E69" s="0" t="inlineStr">
         <is>
           <t>+ полный комплект ( все есть )</t>
         </is>
       </c>
     </row>
-    <row r="70" ht="95.5" customHeight="1" s="12">
-      <c r="A70" s="10" t="inlineStr">
+    <row r="70">
+      <c r="A70" s="0" t="inlineStr">
         <is>
           <t>69</t>
         </is>
       </c>
-      <c r="B70" s="11" t="inlineStr">
-        <is>
-          <t>продам черепаху</t>
-        </is>
-      </c>
-      <c r="C70" s="10" t="inlineStr">
+      <c r="B70" s="0" t="inlineStr">
+        <is>
+          <t>продам черепаху</t>
+        </is>
+      </c>
+      <c r="C70" s="0" t="inlineStr">
         <is>
           <t>02 июля 2022 г.</t>
         </is>
       </c>
-      <c r="D70" s="11" t="inlineStr">
+      <c r="D70" s="0" t="inlineStr">
         <is>
           <t>https://www.olx.kz/d/obyavlenie/prodam-krasnouhuyu-cherepahu-IDmstl9.html#729a76a98a</t>
         </is>
       </c>
-      <c r="E70" s="11" t="inlineStr">
+      <c r="E70" s="0" t="inlineStr">
         <is>
           <t>Красноухая черепаха,самец.,с аквариумом. Причина продажи некому ухаживать.продам.продам</t>
         </is>
       </c>
     </row>
-    <row r="71" ht="41.75" customHeight="1" s="12">
-      <c r="A71" s="10" t="inlineStr">
+    <row r="71">
+      <c r="A71" s="0" t="inlineStr">
         <is>
           <t>70</t>
         </is>
       </c>
-      <c r="B71" s="11" t="inlineStr">
-        <is>
-          <t>продам черепаху</t>
-        </is>
-      </c>
-      <c r="C71" s="10" t="inlineStr">
+      <c r="B71" s="0" t="inlineStr">
+        <is>
+          <t>продам черепаху</t>
+        </is>
+      </c>
+      <c r="C71" s="0" t="inlineStr">
         <is>
           <t>02 июля 2022 г.</t>
         </is>
       </c>
-      <c r="D71" s="11" t="inlineStr">
+      <c r="D71" s="0" t="inlineStr">
         <is>
           <t>https://www.olx.kz/d/obyavlenie/prodam-cherepahu-suhoputnuyu-IDmBYNJ.html#729a76a98a</t>
         </is>
       </c>
-      <c r="E71" s="11" t="inlineStr">
+      <c r="E71" s="0" t="inlineStr">
         <is>
           <t>Продам сухопутную черепаху... порадуйте своих деток...обращаться на ватсап 87085577686</t>
         </is>
@@ -2549,32 +2527,636 @@
       </c>
     </row>
     <row r="74">
-      <c r="A74" t="inlineStr">
+      <c r="A74" s="0" t="inlineStr">
         <is>
           <t>73</t>
         </is>
       </c>
-      <c r="B74" t="inlineStr">
-        <is>
-          <t>продам черепаху</t>
-        </is>
-      </c>
-      <c r="C74" t="inlineStr">
+      <c r="B74" s="0" t="inlineStr">
+        <is>
+          <t>продам черепаху</t>
+        </is>
+      </c>
+      <c r="C74" s="0" t="inlineStr">
         <is>
           <t>01 июля 2022 г.</t>
         </is>
       </c>
-      <c r="D74" t="inlineStr">
+      <c r="D74" s="0" t="inlineStr">
         <is>
           <t>https://www.olx.kz/d/obyavlenie/prodam-vaz-2114-lanzheron-i-cherepaha-isporchennyy-IDmBFY0.html#729a76a98a</t>
         </is>
       </c>
-      <c r="E74" t="inlineStr">
+      <c r="E74" s="0" t="inlineStr">
         <is>
           <t>Продам ваз 2114 без двигатель остальное всё есть шины коробка каса компьютер салон чистый сидений всё хорошие док казак но под залоге стоит</t>
         </is>
       </c>
     </row>
+    <row r="1047973" ht="12.8" customHeight="1" s="8"/>
+    <row r="1047974" ht="12.8" customHeight="1" s="8"/>
+    <row r="1047975" ht="12.8" customHeight="1" s="8"/>
+    <row r="1047976" ht="12.8" customHeight="1" s="8"/>
+    <row r="1047977" ht="12.8" customHeight="1" s="8"/>
+    <row r="1047978" ht="12.8" customHeight="1" s="8"/>
+    <row r="1047979" ht="12.8" customHeight="1" s="8"/>
+    <row r="1047980" ht="12.8" customHeight="1" s="8"/>
+    <row r="1047981" ht="12.8" customHeight="1" s="8"/>
+    <row r="1047982" ht="12.8" customHeight="1" s="8"/>
+    <row r="1047983" ht="12.8" customHeight="1" s="8"/>
+    <row r="1047984" ht="12.8" customHeight="1" s="8"/>
+    <row r="1047985" ht="12.8" customHeight="1" s="8"/>
+    <row r="1047986" ht="12.8" customHeight="1" s="8"/>
+    <row r="1047987" ht="12.8" customHeight="1" s="8"/>
+    <row r="1047988" ht="12.8" customHeight="1" s="8"/>
+    <row r="1047989" ht="12.8" customHeight="1" s="8"/>
+    <row r="1047990" ht="12.8" customHeight="1" s="8"/>
+    <row r="1047991" ht="12.8" customHeight="1" s="8"/>
+    <row r="1047992" ht="12.8" customHeight="1" s="8"/>
+    <row r="1047993" ht="12.8" customHeight="1" s="8"/>
+    <row r="1047994" ht="12.8" customHeight="1" s="8"/>
+    <row r="1047995" ht="12.8" customHeight="1" s="8"/>
+    <row r="1047996" ht="12.8" customHeight="1" s="8"/>
+    <row r="1047997" ht="12.8" customHeight="1" s="8"/>
+    <row r="1047998" ht="12.8" customHeight="1" s="8"/>
+    <row r="1047999" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048000" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048001" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048002" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048003" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048004" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048005" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048006" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048007" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048008" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048009" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048010" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048011" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048012" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048013" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048014" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048015" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048016" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048017" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048018" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048019" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048020" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048021" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048022" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048023" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048024" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048025" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048026" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048027" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048028" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048029" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048030" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048031" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048032" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048033" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048034" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048035" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048036" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048037" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048038" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048039" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048040" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048041" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048042" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048043" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048044" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048045" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048046" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048047" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048048" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048049" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048050" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048051" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048052" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048053" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048054" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048055" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048056" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048057" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048058" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048059" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048060" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048061" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048062" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048063" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048064" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048065" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048066" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048067" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048068" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048069" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048070" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048071" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048072" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048073" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048074" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048075" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048076" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048077" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048078" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048079" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048080" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048081" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048082" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048083" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048084" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048085" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048086" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048087" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048088" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048089" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048090" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048091" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048092" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048093" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048094" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048095" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048096" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048097" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048098" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048099" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048100" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048101" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048102" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048103" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048104" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048105" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048106" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048107" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048108" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048109" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048110" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048111" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048112" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048113" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048114" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048115" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048116" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048117" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048118" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048119" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048120" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048121" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048122" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048123" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048124" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048125" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048126" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048127" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048128" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048129" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048130" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048131" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048132" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048133" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048134" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048135" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048136" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048137" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048138" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048139" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048140" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048141" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048142" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048143" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048144" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048145" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048146" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048147" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048148" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048149" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048150" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048151" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048152" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048153" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048154" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048155" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048156" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048157" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048158" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048159" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048160" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048161" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048162" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048163" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048164" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048165" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048166" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048167" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048168" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048169" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048170" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048171" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048172" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048173" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048174" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048175" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048176" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048177" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048178" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048179" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048180" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048181" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048182" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048183" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048184" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048185" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048186" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048187" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048188" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048189" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048190" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048191" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048192" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048193" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048194" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048195" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048196" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048197" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048198" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048199" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048200" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048201" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048202" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048203" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048204" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048205" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048206" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048207" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048208" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048209" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048210" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048211" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048212" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048213" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048214" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048215" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048216" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048217" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048218" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048219" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048220" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048221" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048222" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048223" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048224" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048225" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048226" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048227" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048228" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048229" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048230" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048231" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048232" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048233" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048234" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048235" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048236" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048237" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048238" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048239" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048240" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048241" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048242" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048243" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048244" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048245" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048246" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048247" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048248" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048249" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048250" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048251" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048252" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048253" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048254" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048255" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048256" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048257" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048258" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048259" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048260" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048261" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048262" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048263" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048264" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048265" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048266" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048267" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048268" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048269" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048270" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048271" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048272" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048273" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048274" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048275" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048276" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048277" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048278" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048279" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048280" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048281" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048282" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048283" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048284" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048285" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048286" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048287" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048288" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048289" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048290" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048291" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048292" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048293" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048294" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048295" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048296" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048297" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048298" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048299" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048300" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048301" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048302" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048303" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048304" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048305" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048306" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048307" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048308" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048309" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048310" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048311" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048312" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048313" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048314" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048315" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048316" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048317" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048318" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048319" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048320" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048321" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048322" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048323" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048324" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048325" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048326" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048327" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048328" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048329" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048330" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048331" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048332" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048333" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048334" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048335" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048336" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048337" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048338" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048339" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048340" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048341" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048342" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048343" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048344" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048345" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048346" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048347" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048348" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048349" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048350" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048351" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048352" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048353" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048354" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048355" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048356" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048357" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048358" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048359" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048360" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048361" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048362" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048363" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048364" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048365" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048366" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048367" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048368" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048369" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048370" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048371" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048372" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048373" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048374" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048375" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048376" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048377" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048378" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048379" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048380" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048381" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048382" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048383" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048384" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048385" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048386" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048387" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048388" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048389" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048390" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048391" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048392" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048393" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048394" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048395" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048396" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048397" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048398" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048399" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048400" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048401" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048402" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048403" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048404" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048405" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048406" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048407" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048408" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048409" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048410" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048411" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048412" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048413" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048414" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048415" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048416" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048417" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048418" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048419" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048420" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048421" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048422" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048423" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048424" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048425" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048426" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048427" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048428" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048429" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048430" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048431" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048432" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048433" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048434" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048435" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048436" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048437" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048438" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048439" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048440" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048441" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048442" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048443" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048444" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048445" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048446" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048447" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048448" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048449" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048450" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048451" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048452" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048453" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048454" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048455" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048456" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048457" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048458" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048459" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048460" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048461" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048462" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048463" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048464" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048465" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048466" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048467" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048468" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048469" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048470" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048471" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048472" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048473" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048474" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048475" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048476" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048477" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048478" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048479" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048480" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048481" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048482" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048483" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048484" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048485" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048486" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048487" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048488" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048489" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048490" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048491" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048492" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048493" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048494" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048495" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048496" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048497" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048498" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048499" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048500" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048501" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048502" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048503" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048504" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048505" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048506" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048507" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048508" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048509" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048510" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048511" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048512" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048513" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048514" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048515" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048516" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048517" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048518" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048519" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048520" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048521" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048522" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048523" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048524" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048525" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048526" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048527" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048528" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048529" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048530" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048531" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048532" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048533" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048534" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048535" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048536" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048537" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048538" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048539" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048540" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048541" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048542" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048543" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048544" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048545" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048546" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048547" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048548" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048549" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048550" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048551" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048552" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048553" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048554" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048555" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048556" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048557" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048558" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048559" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048560" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048561" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048562" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048563" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048564" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048565" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048566" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048567" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048568" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048569" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048570" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048571" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048572" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048573" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048574" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048575" ht="12.8" customHeight="1" s="8"/>
+    <row r="1048576" ht="12.8" customHeight="1" s="8"/>
   </sheetData>
   <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>